<commit_message>
updated simple finance lessons
</commit_message>
<xml_diff>
--- a/content/docs/simple_financial_model.xlsx
+++ b/content/docs/simple_financial_model.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27710"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="2780" windowWidth="35220" windowHeight="18380" tabRatio="293"/>
+    <workbookView xWindow="1700" yWindow="2780" windowWidth="35220" windowHeight="18380" tabRatio="293" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Model &quot;Paid Engine&quot;" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>Customers</t>
   </si>
@@ -187,6 +190,9 @@
   </si>
   <si>
     <t>Dec</t>
+  </si>
+  <si>
+    <t>Change in month churn each month</t>
   </si>
 </sst>
 </file>
@@ -198,7 +204,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -429,7 +435,6 @@
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -440,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="106"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -457,6 +462,7 @@
     <xf numFmtId="6" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="107" applyFont="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -718,11 +724,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2108560224"/>
-        <c:axId val="-2129986192"/>
+        <c:axId val="-110499984"/>
+        <c:axId val="-110499456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2108560224"/>
+        <c:axId val="-110499984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -731,7 +737,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129986192"/>
+        <c:crossAx val="-110499456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -739,7 +745,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129986192"/>
+        <c:axId val="-110499456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -750,7 +756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108560224"/>
+        <c:crossAx val="-110499984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -825,76 +831,76 @@
                 <c:formatCode>"$"#,##0_);[Red]\("$"#,##0\)</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>100000.0</c:v>
+                  <c:v>150000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71200.0</c:v>
+                  <c:v>121200.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46537.0</c:v>
+                  <c:v>95938.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26022.55</c:v>
+                  <c:v>73829.8809375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9737.618650000003</c:v>
+                  <c:v>54677.55284217773</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2170.464559999993</c:v>
+                  <c:v>38419.52455027811</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-9489.263606689987</c:v>
+                  <c:v>25094.01953996541</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-11940.87456374688</c:v>
+                  <c:v>14817.74625625217</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-9180.068879721097</c:v>
+                  <c:v>7772.328433356666</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-791.0046535529472</c:v>
+                  <c:v>4196.11746817955</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13717.48047401458</c:v>
+                  <c:v>4379.644519076417</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34918.02633374944</c:v>
+                  <c:v>8663.605703622012</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>63201.42868812692</c:v>
+                  <c:v>17438.67053524661</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96239.22230947827</c:v>
+                  <c:v>31146.65543387868</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>134425.8451866921</c:v>
+                  <c:v>50282.76641398878</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>178541.8852268389</c:v>
+                  <c:v>75398.7214076335</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>229426.1721432059</c:v>
+                  <c:v>107106.6336106824</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>287988.6752082669</c:v>
+                  <c:v>146083.5854573999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>355224.066373612</c:v>
+                  <c:v>193076.85632573</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>432226.2620539597</c:v>
+                  <c:v>248909.790948335</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>520204.2594633877</c:v>
+                  <c:v>314488.313043337</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>620499.597032417</c:v>
+                  <c:v>390808.1020367817</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>734605.7926396502</c:v>
+                  <c:v>478962.4613534566</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>864190.1481993822</c:v>
+                  <c:v>580150.9155633064</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -910,11 +916,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2129928608"/>
-        <c:axId val="-2129925776"/>
+        <c:axId val="-110474848"/>
+        <c:axId val="-110472528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2129928608"/>
+        <c:axId val="-110474848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -923,7 +929,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129925776"/>
+        <c:crossAx val="-110472528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -931,7 +937,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129925776"/>
+        <c:axId val="-110472528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300000.0"/>
@@ -943,7 +949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129928608"/>
+        <c:crossAx val="-110474848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1011,73 +1017,73 @@
                   <c:v>-28800.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-24663.0</c:v>
+                  <c:v>-25261.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-20514.45</c:v>
+                  <c:v>-22108.6190625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-16284.93135</c:v>
+                  <c:v>-19152.32809532226</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-11908.08321</c:v>
+                  <c:v>-16258.02829189962</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-7318.799046689993</c:v>
+                  <c:v>-13325.50501031271</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2451.610957056895</c:v>
+                  <c:v>-10276.27328371324</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2760.805684025785</c:v>
+                  <c:v>-7045.417822895502</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8389.06422616815</c:v>
+                  <c:v>-3576.210965177117</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14508.48512756752</c:v>
+                  <c:v>183.5270508968679</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21200.54585973486</c:v>
+                  <c:v>4283.961184545594</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28283.40235437749</c:v>
+                  <c:v>8775.064831624601</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>33037.79362135133</c:v>
+                  <c:v>13707.98489863206</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>38186.62287721384</c:v>
+                  <c:v>19136.1109801101</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44116.04004014677</c:v>
+                  <c:v>25115.95499364474</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50884.28691636702</c:v>
+                  <c:v>31707.91220304885</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>58562.50306506103</c:v>
+                  <c:v>38976.95184671752</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>67235.3911653451</c:v>
+                  <c:v>46993.27086833013</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>77002.19568034766</c:v>
+                  <c:v>55832.934622605</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>87977.99740942793</c:v>
+                  <c:v>65578.522095002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>100295.3375690293</c:v>
+                  <c:v>76319.7889934447</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>114106.1956072332</c:v>
+                  <c:v>88154.3593166749</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>129584.355559732</c:v>
+                  <c:v>101188.4542098498</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>146115.2850932348</c:v>
+                  <c:v>115537.6657786386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1093,11 +1099,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2129894992"/>
-        <c:axId val="-2129771600"/>
+        <c:axId val="-110451904"/>
+        <c:axId val="-110449152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2129894992"/>
+        <c:axId val="-110451904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1106,7 +1112,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129771600"/>
+        <c:crossAx val="-110449152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1114,7 +1120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129771600"/>
+        <c:axId val="-110449152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100000.0"/>
@@ -1126,7 +1132,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2129894992"/>
+        <c:crossAx val="-110451904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1567,860 +1573,860 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" style="15" customWidth="1"/>
-    <col min="2" max="25" width="10" style="15" customWidth="1"/>
-    <col min="26" max="16384" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="31.83203125" style="14" customWidth="1"/>
+    <col min="2" max="25" width="10" style="14" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="O2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="P2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="26" t="s">
+      <c r="S2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="26" t="s">
+      <c r="T2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="U2" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="V2" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="W2" s="26" t="s">
+      <c r="W2" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="X2" s="26" t="s">
+      <c r="X2" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Y2" s="26" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <v>100</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <f>B3*(1+B4)</f>
         <v>150</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <f t="shared" ref="D3:Y3" si="0">C3*(1+C4)</f>
         <v>225</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <f t="shared" si="0"/>
         <v>315</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <f t="shared" si="0"/>
         <v>441</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <f t="shared" si="0"/>
         <v>573.30000000000007</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <f t="shared" si="0"/>
         <v>745.29000000000008</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="15">
         <f t="shared" si="0"/>
         <v>968.87700000000018</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="15">
         <f t="shared" si="0"/>
         <v>1259.5401000000002</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="15">
         <f t="shared" si="0"/>
         <v>1511.4481200000002</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="15">
         <f t="shared" si="0"/>
         <v>1813.7377440000002</v>
       </c>
-      <c r="M3" s="23">
+      <c r="M3" s="22">
         <f t="shared" si="0"/>
         <v>1995.1115184000005</v>
       </c>
-      <c r="N3" s="16">
+      <c r="N3" s="15">
         <f t="shared" si="0"/>
         <v>2194.6226702400008</v>
       </c>
-      <c r="O3" s="16">
+      <c r="O3" s="15">
         <f t="shared" si="0"/>
         <v>2304.3538037520011</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="15">
         <f t="shared" si="0"/>
         <v>2419.5714939396012</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3" s="15">
         <f t="shared" si="0"/>
         <v>2540.5500686365813</v>
       </c>
-      <c r="R3" s="16">
+      <c r="R3" s="15">
         <f t="shared" si="0"/>
         <v>2667.5775720684105</v>
       </c>
-      <c r="S3" s="16">
+      <c r="S3" s="15">
         <f t="shared" si="0"/>
         <v>2800.9564506718311</v>
       </c>
-      <c r="T3" s="16">
+      <c r="T3" s="15">
         <f t="shared" si="0"/>
         <v>2941.004273205423</v>
       </c>
-      <c r="U3" s="16">
+      <c r="U3" s="15">
         <f t="shared" si="0"/>
         <v>3088.0544868656943</v>
       </c>
-      <c r="V3" s="16">
+      <c r="V3" s="15">
         <f t="shared" si="0"/>
         <v>3242.4572112089791</v>
       </c>
-      <c r="W3" s="16">
+      <c r="W3" s="15">
         <f t="shared" si="0"/>
         <v>3404.5800717694283</v>
       </c>
-      <c r="X3" s="16">
+      <c r="X3" s="15">
         <f t="shared" si="0"/>
         <v>3574.8090753578999</v>
       </c>
-      <c r="Y3" s="23">
+      <c r="Y3" s="22">
         <f t="shared" si="0"/>
         <v>3753.5495291257953</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>0.5</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <v>0.5</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>0.4</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>0.4</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>0.3</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>0.3</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <v>0.3</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="16">
         <v>0.3</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="16">
         <v>0.2</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="16">
         <v>0.2</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="16">
         <v>0.1</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="23">
         <v>0.1</v>
       </c>
-      <c r="N4" s="17">
+      <c r="N4" s="16">
         <v>0.05</v>
       </c>
-      <c r="O4" s="17">
+      <c r="O4" s="16">
         <v>0.05</v>
       </c>
-      <c r="P4" s="17">
+      <c r="P4" s="16">
         <v>0.05</v>
       </c>
-      <c r="Q4" s="17">
+      <c r="Q4" s="16">
         <v>0.05</v>
       </c>
-      <c r="R4" s="17">
+      <c r="R4" s="16">
         <v>0.05</v>
       </c>
-      <c r="S4" s="17">
+      <c r="S4" s="16">
         <v>0.05</v>
       </c>
-      <c r="T4" s="17">
+      <c r="T4" s="16">
         <v>0.05</v>
       </c>
-      <c r="U4" s="17">
+      <c r="U4" s="16">
         <v>0.05</v>
       </c>
-      <c r="V4" s="17">
+      <c r="V4" s="16">
         <v>0.05</v>
       </c>
-      <c r="W4" s="17">
+      <c r="W4" s="16">
         <v>0.05</v>
       </c>
-      <c r="X4" s="17">
+      <c r="X4" s="16">
         <v>0.05</v>
       </c>
-      <c r="Y4" s="24">
+      <c r="Y4" s="23">
         <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="18">
-        <f>B3*$D$16</f>
+      <c r="B5" s="17">
+        <f t="shared" ref="B5:Y5" si="1">B3*$D$16</f>
         <v>495</v>
       </c>
-      <c r="C5" s="18">
-        <f>C3*$D$16</f>
+      <c r="C5" s="17">
+        <f t="shared" si="1"/>
         <v>742.5</v>
       </c>
-      <c r="D5" s="18">
-        <f>D3*$D$16</f>
+      <c r="D5" s="17">
+        <f t="shared" si="1"/>
         <v>1113.75</v>
       </c>
-      <c r="E5" s="18">
-        <f>E3*$D$16</f>
+      <c r="E5" s="17">
+        <f t="shared" si="1"/>
         <v>1559.25</v>
       </c>
-      <c r="F5" s="18">
-        <f>F3*$D$16</f>
+      <c r="F5" s="17">
+        <f t="shared" si="1"/>
         <v>2182.9500000000003</v>
       </c>
-      <c r="G5" s="18">
-        <f>G3*$D$16</f>
+      <c r="G5" s="17">
+        <f t="shared" si="1"/>
         <v>2837.8350000000005</v>
       </c>
-      <c r="H5" s="18">
-        <f>H3*$D$16</f>
+      <c r="H5" s="17">
+        <f t="shared" si="1"/>
         <v>3689.1855000000005</v>
       </c>
-      <c r="I5" s="18">
-        <f>I3*$D$16</f>
+      <c r="I5" s="17">
+        <f t="shared" si="1"/>
         <v>4795.9411500000015</v>
       </c>
-      <c r="J5" s="18">
-        <f>J3*$D$16</f>
+      <c r="J5" s="17">
+        <f t="shared" si="1"/>
         <v>6234.7234950000011</v>
       </c>
-      <c r="K5" s="18">
-        <f>K3*$D$16</f>
+      <c r="K5" s="17">
+        <f t="shared" si="1"/>
         <v>7481.6681940000017</v>
       </c>
-      <c r="L5" s="18">
-        <f>L3*$D$16</f>
+      <c r="L5" s="17">
+        <f t="shared" si="1"/>
         <v>8978.0018328000024</v>
       </c>
-      <c r="M5" s="25">
-        <f>M3*$D$16</f>
+      <c r="M5" s="24">
+        <f t="shared" si="1"/>
         <v>9875.8020160800024</v>
       </c>
-      <c r="N5" s="18">
-        <f>N3*$D$16</f>
+      <c r="N5" s="17">
+        <f t="shared" si="1"/>
         <v>10863.382217688004</v>
       </c>
-      <c r="O5" s="18">
-        <f>O3*$D$16</f>
+      <c r="O5" s="17">
+        <f t="shared" si="1"/>
         <v>11406.551328572406</v>
       </c>
-      <c r="P5" s="18">
-        <f>P3*$D$16</f>
+      <c r="P5" s="17">
+        <f t="shared" si="1"/>
         <v>11976.878895001026</v>
       </c>
-      <c r="Q5" s="18">
-        <f>Q3*$D$16</f>
+      <c r="Q5" s="17">
+        <f t="shared" si="1"/>
         <v>12575.722839751077</v>
       </c>
-      <c r="R5" s="18">
-        <f>R3*$D$16</f>
+      <c r="R5" s="17">
+        <f t="shared" si="1"/>
         <v>13204.508981738632</v>
       </c>
-      <c r="S5" s="18">
-        <f>S3*$D$16</f>
+      <c r="S5" s="17">
+        <f t="shared" si="1"/>
         <v>13864.734430825565</v>
       </c>
-      <c r="T5" s="18">
-        <f>T3*$D$16</f>
+      <c r="T5" s="17">
+        <f t="shared" si="1"/>
         <v>14557.971152366845</v>
       </c>
-      <c r="U5" s="18">
-        <f>U3*$D$16</f>
+      <c r="U5" s="17">
+        <f t="shared" si="1"/>
         <v>15285.869709985187</v>
       </c>
-      <c r="V5" s="18">
-        <f>V3*$D$16</f>
+      <c r="V5" s="17">
+        <f t="shared" si="1"/>
         <v>16050.163195484447</v>
       </c>
-      <c r="W5" s="18">
-        <f>W3*$D$16</f>
+      <c r="W5" s="17">
+        <f t="shared" si="1"/>
         <v>16852.67135525867</v>
       </c>
-      <c r="X5" s="18">
-        <f>X3*$D$16</f>
+      <c r="X5" s="17">
+        <f t="shared" si="1"/>
         <v>17695.304923021606</v>
       </c>
-      <c r="Y5" s="25">
-        <f>Y3*$D$16</f>
+      <c r="Y5" s="24">
+        <f t="shared" si="1"/>
         <v>18580.070169172686</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>1</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>1</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>1</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <v>2</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="14">
         <v>2</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>2</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="14">
         <v>2</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="14">
         <v>2</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="14">
         <v>2</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="14">
         <v>3</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="21">
         <v>3</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="14">
         <v>3</v>
       </c>
-      <c r="O6" s="15">
+      <c r="O6" s="14">
         <v>3</v>
       </c>
-      <c r="P6" s="15">
+      <c r="P6" s="14">
         <v>3</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="14">
         <v>3</v>
       </c>
-      <c r="R6" s="15">
+      <c r="R6" s="14">
         <v>3</v>
       </c>
-      <c r="S6" s="15">
+      <c r="S6" s="14">
         <v>3</v>
       </c>
-      <c r="T6" s="15">
+      <c r="T6" s="14">
         <v>3</v>
       </c>
-      <c r="U6" s="15">
+      <c r="U6" s="14">
         <v>3</v>
       </c>
-      <c r="V6" s="15">
+      <c r="V6" s="14">
         <v>3</v>
       </c>
-      <c r="W6" s="15">
+      <c r="W6" s="14">
         <v>3</v>
       </c>
-      <c r="X6" s="15">
+      <c r="X6" s="14">
         <v>3</v>
       </c>
-      <c r="Y6" s="22">
+      <c r="Y6" s="21">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18">
-        <f>B6*$D$18</f>
+      <c r="B7" s="17">
+        <f t="shared" ref="B7:Y7" si="2">B6*$D$18</f>
         <v>4166.666666666667</v>
       </c>
-      <c r="C7" s="18">
-        <f>C6*$D$18</f>
+      <c r="C7" s="17">
+        <f t="shared" si="2"/>
         <v>4166.666666666667</v>
       </c>
-      <c r="D7" s="18">
-        <f>D6*$D$18</f>
+      <c r="D7" s="17">
+        <f t="shared" si="2"/>
         <v>4166.666666666667</v>
       </c>
-      <c r="E7" s="18">
-        <f>E6*$D$18</f>
+      <c r="E7" s="17">
+        <f t="shared" si="2"/>
         <v>4166.666666666667</v>
       </c>
-      <c r="F7" s="18">
-        <f>F6*$D$18</f>
+      <c r="F7" s="17">
+        <f t="shared" si="2"/>
         <v>8333.3333333333339</v>
       </c>
-      <c r="G7" s="18">
-        <f>G6*$D$18</f>
+      <c r="G7" s="17">
+        <f t="shared" si="2"/>
         <v>8333.3333333333339</v>
       </c>
-      <c r="H7" s="18">
-        <f>H6*$D$18</f>
+      <c r="H7" s="17">
+        <f t="shared" si="2"/>
         <v>8333.3333333333339</v>
       </c>
-      <c r="I7" s="18">
-        <f>I6*$D$18</f>
+      <c r="I7" s="17">
+        <f t="shared" si="2"/>
         <v>8333.3333333333339</v>
       </c>
-      <c r="J7" s="18">
-        <f>J6*$D$18</f>
+      <c r="J7" s="17">
+        <f t="shared" si="2"/>
         <v>8333.3333333333339</v>
       </c>
-      <c r="K7" s="18">
-        <f>K6*$D$18</f>
+      <c r="K7" s="17">
+        <f t="shared" si="2"/>
         <v>8333.3333333333339</v>
       </c>
-      <c r="L7" s="18">
-        <f>L6*$D$18</f>
+      <c r="L7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="M7" s="25">
-        <f>M6*$D$18</f>
+      <c r="M7" s="24">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="N7" s="18">
-        <f>N6*$D$18</f>
+      <c r="N7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="O7" s="18">
-        <f>O6*$D$18</f>
+      <c r="O7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="P7" s="18">
-        <f>P6*$D$18</f>
+      <c r="P7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="Q7" s="18">
-        <f>Q6*$D$18</f>
+      <c r="Q7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="R7" s="18">
-        <f>R6*$D$18</f>
+      <c r="R7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="S7" s="18">
-        <f>S6*$D$18</f>
+      <c r="S7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="T7" s="18">
-        <f>T6*$D$18</f>
+      <c r="T7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="U7" s="18">
-        <f>U6*$D$18</f>
+      <c r="U7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="V7" s="18">
-        <f>V6*$D$18</f>
+      <c r="V7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="W7" s="18">
-        <f>W6*$D$18</f>
+      <c r="W7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="X7" s="18">
-        <f>X6*$D$18</f>
+      <c r="X7" s="17">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="Y7" s="25">
-        <f>Y6*$D$18</f>
+      <c r="Y7" s="24">
+        <f t="shared" si="2"/>
         <v>12500</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="18">
-        <f>B7+$D$19</f>
+      <c r="B8" s="17">
+        <f t="shared" ref="B8:Y8" si="3">B7+$D$19</f>
         <v>5166.666666666667</v>
       </c>
-      <c r="C8" s="18">
-        <f>C7+$D$19</f>
+      <c r="C8" s="17">
+        <f t="shared" si="3"/>
         <v>5166.666666666667</v>
       </c>
-      <c r="D8" s="18">
-        <f>D7+$D$19</f>
+      <c r="D8" s="17">
+        <f t="shared" si="3"/>
         <v>5166.666666666667</v>
       </c>
-      <c r="E8" s="18">
-        <f>E7+$D$19</f>
+      <c r="E8" s="17">
+        <f t="shared" si="3"/>
         <v>5166.666666666667</v>
       </c>
-      <c r="F8" s="18">
-        <f>F7+$D$19</f>
+      <c r="F8" s="17">
+        <f t="shared" si="3"/>
         <v>9333.3333333333339</v>
       </c>
-      <c r="G8" s="18">
-        <f>G7+$D$19</f>
+      <c r="G8" s="17">
+        <f t="shared" si="3"/>
         <v>9333.3333333333339</v>
       </c>
-      <c r="H8" s="18">
-        <f>H7+$D$19</f>
+      <c r="H8" s="17">
+        <f t="shared" si="3"/>
         <v>9333.3333333333339</v>
       </c>
-      <c r="I8" s="18">
-        <f>I7+$D$19</f>
+      <c r="I8" s="17">
+        <f t="shared" si="3"/>
         <v>9333.3333333333339</v>
       </c>
-      <c r="J8" s="18">
-        <f>J7+$D$19</f>
+      <c r="J8" s="17">
+        <f t="shared" si="3"/>
         <v>9333.3333333333339</v>
       </c>
-      <c r="K8" s="18">
-        <f>K7+$D$19</f>
+      <c r="K8" s="17">
+        <f t="shared" si="3"/>
         <v>9333.3333333333339</v>
       </c>
-      <c r="L8" s="18">
-        <f>L7+$D$19</f>
+      <c r="L8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="M8" s="25">
-        <f>M7+$D$19</f>
+      <c r="M8" s="24">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="N8" s="18">
-        <f>N7+$D$19</f>
+      <c r="N8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="O8" s="18">
-        <f>O7+$D$19</f>
+      <c r="O8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="P8" s="18">
-        <f>P7+$D$19</f>
+      <c r="P8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="Q8" s="18">
-        <f>Q7+$D$19</f>
+      <c r="Q8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="R8" s="18">
-        <f>R7+$D$19</f>
+      <c r="R8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="S8" s="18">
-        <f>S7+$D$19</f>
+      <c r="S8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="T8" s="18">
-        <f>T7+$D$19</f>
+      <c r="T8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="U8" s="18">
-        <f>U7+$D$19</f>
+      <c r="U8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="V8" s="18">
-        <f>V7+$D$19</f>
+      <c r="V8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="W8" s="18">
-        <f>W7+$D$19</f>
+      <c r="W8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="X8" s="18">
-        <f>X7+$D$19</f>
+      <c r="X8" s="17">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
-      <c r="Y8" s="25">
-        <f>Y7+$D$19</f>
+      <c r="Y8" s="24">
+        <f t="shared" si="3"/>
         <v>13500</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="17">
         <f>B5-B8</f>
         <v>-4671.666666666667</v>
       </c>
-      <c r="C9" s="18">
-        <f t="shared" ref="C9:H9" si="1">C5-C8</f>
+      <c r="C9" s="17">
+        <f t="shared" ref="C9:H9" si="4">C5-C8</f>
         <v>-4424.166666666667</v>
       </c>
-      <c r="D9" s="18">
-        <f t="shared" si="1"/>
+      <c r="D9" s="17">
+        <f t="shared" si="4"/>
         <v>-4052.916666666667</v>
       </c>
-      <c r="E9" s="18">
-        <f t="shared" si="1"/>
+      <c r="E9" s="17">
+        <f t="shared" si="4"/>
         <v>-3607.416666666667</v>
       </c>
-      <c r="F9" s="18">
-        <f t="shared" si="1"/>
+      <c r="F9" s="17">
+        <f t="shared" si="4"/>
         <v>-7150.3833333333332</v>
       </c>
-      <c r="G9" s="18">
-        <f t="shared" si="1"/>
+      <c r="G9" s="17">
+        <f t="shared" si="4"/>
         <v>-6495.498333333333</v>
       </c>
-      <c r="H9" s="18">
-        <f t="shared" si="1"/>
+      <c r="H9" s="17">
+        <f t="shared" si="4"/>
         <v>-5644.1478333333334</v>
       </c>
-      <c r="I9" s="18">
-        <f t="shared" ref="I9" si="2">I5-I8</f>
+      <c r="I9" s="17">
+        <f t="shared" ref="I9" si="5">I5-I8</f>
         <v>-4537.3921833333325</v>
       </c>
-      <c r="J9" s="18">
-        <f t="shared" ref="J9" si="3">J5-J8</f>
+      <c r="J9" s="17">
+        <f t="shared" ref="J9" si="6">J5-J8</f>
         <v>-3098.6098383333328</v>
       </c>
-      <c r="K9" s="18">
-        <f t="shared" ref="K9" si="4">K5-K8</f>
+      <c r="K9" s="17">
+        <f t="shared" ref="K9" si="7">K5-K8</f>
         <v>-1851.6651393333323</v>
       </c>
-      <c r="L9" s="18">
-        <f t="shared" ref="L9" si="5">L5-L8</f>
+      <c r="L9" s="17">
+        <f t="shared" ref="L9" si="8">L5-L8</f>
         <v>-4521.9981671999976</v>
       </c>
-      <c r="M9" s="25">
-        <f t="shared" ref="M9:N9" si="6">M5-M8</f>
+      <c r="M9" s="24">
+        <f t="shared" ref="M9:N9" si="9">M5-M8</f>
         <v>-3624.1979839199976</v>
       </c>
-      <c r="N9" s="18">
-        <f t="shared" si="6"/>
+      <c r="N9" s="17">
+        <f t="shared" si="9"/>
         <v>-2636.6177823119961</v>
       </c>
-      <c r="O9" s="18">
-        <f t="shared" ref="O9" si="7">O5-O8</f>
+      <c r="O9" s="17">
+        <f t="shared" ref="O9" si="10">O5-O8</f>
         <v>-2093.4486714275936</v>
       </c>
-      <c r="P9" s="18">
-        <f t="shared" ref="P9" si="8">P5-P8</f>
+      <c r="P9" s="17">
+        <f t="shared" ref="P9" si="11">P5-P8</f>
         <v>-1523.1211049989743</v>
       </c>
-      <c r="Q9" s="18">
-        <f t="shared" ref="Q9" si="9">Q5-Q8</f>
+      <c r="Q9" s="17">
+        <f t="shared" ref="Q9" si="12">Q5-Q8</f>
         <v>-924.27716024892288</v>
       </c>
-      <c r="R9" s="18">
-        <f t="shared" ref="R9" si="10">R5-R8</f>
+      <c r="R9" s="17">
+        <f t="shared" ref="R9" si="13">R5-R8</f>
         <v>-295.49101826136757</v>
       </c>
-      <c r="S9" s="18">
-        <f t="shared" ref="S9" si="11">S5-S8</f>
+      <c r="S9" s="17">
+        <f t="shared" ref="S9" si="14">S5-S8</f>
         <v>364.73443082556514</v>
       </c>
-      <c r="T9" s="18">
-        <f t="shared" ref="T9" si="12">T5-T8</f>
+      <c r="T9" s="17">
+        <f t="shared" ref="T9" si="15">T5-T8</f>
         <v>1057.9711523668448</v>
       </c>
-      <c r="U9" s="18">
-        <f t="shared" ref="U9" si="13">U5-U8</f>
+      <c r="U9" s="17">
+        <f t="shared" ref="U9" si="16">U5-U8</f>
         <v>1785.869709985187</v>
       </c>
-      <c r="V9" s="18">
-        <f t="shared" ref="V9" si="14">V5-V8</f>
+      <c r="V9" s="17">
+        <f t="shared" ref="V9" si="17">V5-V8</f>
         <v>2550.163195484447</v>
       </c>
-      <c r="W9" s="18">
-        <f t="shared" ref="W9" si="15">W5-W8</f>
+      <c r="W9" s="17">
+        <f t="shared" ref="W9" si="18">W5-W8</f>
         <v>3352.6713552586698</v>
       </c>
-      <c r="X9" s="18">
-        <f t="shared" ref="X9" si="16">X5-X8</f>
+      <c r="X9" s="17">
+        <f t="shared" ref="X9" si="19">X5-X8</f>
         <v>4195.3049230216056</v>
       </c>
-      <c r="Y9" s="25">
-        <f t="shared" ref="Y9" si="17">Y5-Y8</f>
+      <c r="Y9" s="24">
+        <f t="shared" ref="Y9" si="20">Y5-Y8</f>
         <v>5080.0701691726863</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <f>D20+B9</f>
         <v>45328.333333333336</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <f>B10+C9</f>
         <v>40904.166666666672</v>
       </c>
-      <c r="D10" s="18">
-        <f t="shared" ref="D10:H10" si="18">C10+D9</f>
+      <c r="D10" s="17">
+        <f t="shared" ref="D10:H10" si="21">C10+D9</f>
         <v>36851.250000000007</v>
       </c>
-      <c r="E10" s="18">
-        <f t="shared" si="18"/>
+      <c r="E10" s="17">
+        <f t="shared" si="21"/>
         <v>33243.833333333343</v>
       </c>
-      <c r="F10" s="18">
-        <f t="shared" si="18"/>
+      <c r="F10" s="17">
+        <f t="shared" si="21"/>
         <v>26093.450000000012</v>
       </c>
-      <c r="G10" s="18">
-        <f t="shared" si="18"/>
+      <c r="G10" s="17">
+        <f t="shared" si="21"/>
         <v>19597.951666666679</v>
       </c>
-      <c r="H10" s="18">
-        <f t="shared" si="18"/>
+      <c r="H10" s="17">
+        <f t="shared" si="21"/>
         <v>13953.803833333346</v>
       </c>
-      <c r="I10" s="18">
-        <f t="shared" ref="I10" si="19">H10+I9</f>
+      <c r="I10" s="17">
+        <f t="shared" ref="I10" si="22">H10+I9</f>
         <v>9416.4116500000127</v>
       </c>
-      <c r="J10" s="18">
-        <f t="shared" ref="J10" si="20">I10+J9</f>
+      <c r="J10" s="17">
+        <f t="shared" ref="J10" si="23">I10+J9</f>
         <v>6317.8018116666799</v>
       </c>
-      <c r="K10" s="18">
-        <f t="shared" ref="K10" si="21">J10+K9</f>
+      <c r="K10" s="17">
+        <f t="shared" ref="K10" si="24">J10+K9</f>
         <v>4466.1366723333476</v>
       </c>
-      <c r="L10" s="18">
-        <f t="shared" ref="L10" si="22">K10+L9</f>
+      <c r="L10" s="17">
+        <f t="shared" ref="L10" si="25">K10+L9</f>
         <v>-55.861494866649991</v>
       </c>
-      <c r="M10" s="25">
-        <f t="shared" ref="M10:N10" si="23">L10+M9</f>
+      <c r="M10" s="24">
+        <f t="shared" ref="M10:N10" si="26">L10+M9</f>
         <v>-3680.0594787866476</v>
       </c>
-      <c r="N10" s="18">
-        <f t="shared" si="23"/>
+      <c r="N10" s="17">
+        <f t="shared" si="26"/>
         <v>-6316.6772610986436</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10" s="17">
         <f>N10+O9</f>
         <v>-8410.1259325262363</v>
       </c>
-      <c r="P10" s="18">
-        <f t="shared" ref="P10" si="24">O10+P9</f>
+      <c r="P10" s="17">
+        <f t="shared" ref="P10" si="27">O10+P9</f>
         <v>-9933.2470375252105</v>
       </c>
-      <c r="Q10" s="18">
-        <f t="shared" ref="Q10" si="25">P10+Q9</f>
+      <c r="Q10" s="17">
+        <f t="shared" ref="Q10" si="28">P10+Q9</f>
         <v>-10857.524197774133</v>
       </c>
-      <c r="R10" s="18">
-        <f t="shared" ref="R10" si="26">Q10+R9</f>
+      <c r="R10" s="17">
+        <f t="shared" ref="R10" si="29">Q10+R9</f>
         <v>-11153.015216035501</v>
       </c>
-      <c r="S10" s="18">
-        <f t="shared" ref="S10" si="27">R10+S9</f>
+      <c r="S10" s="17">
+        <f t="shared" ref="S10" si="30">R10+S9</f>
         <v>-10788.280785209936</v>
       </c>
-      <c r="T10" s="18">
-        <f t="shared" ref="T10" si="28">S10+T9</f>
+      <c r="T10" s="17">
+        <f t="shared" ref="T10" si="31">S10+T9</f>
         <v>-9730.3096328430911</v>
       </c>
-      <c r="U10" s="18">
-        <f t="shared" ref="U10" si="29">T10+U9</f>
+      <c r="U10" s="17">
+        <f t="shared" ref="U10" si="32">T10+U9</f>
         <v>-7944.4399228579041</v>
       </c>
-      <c r="V10" s="18">
-        <f t="shared" ref="V10" si="30">U10+V9</f>
+      <c r="V10" s="17">
+        <f t="shared" ref="V10" si="33">U10+V9</f>
         <v>-5394.2767273734571</v>
       </c>
-      <c r="W10" s="18">
-        <f t="shared" ref="W10" si="31">V10+W9</f>
+      <c r="W10" s="17">
+        <f t="shared" ref="W10" si="34">V10+W9</f>
         <v>-2041.6053721147873</v>
       </c>
-      <c r="X10" s="18">
-        <f t="shared" ref="X10" si="32">W10+X9</f>
+      <c r="X10" s="17">
+        <f t="shared" ref="X10" si="35">W10+X9</f>
         <v>2153.6995509068183</v>
       </c>
-      <c r="Y10" s="25">
-        <f t="shared" ref="Y10" si="33">X10+Y9</f>
+      <c r="Y10" s="24">
+        <f t="shared" ref="Y10" si="36">X10+Y9</f>
         <v>7233.7697200795046</v>
       </c>
     </row>
@@ -2428,57 +2434,57 @@
     <row r="12" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="17"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="18">
         <v>4.95</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="17">
         <v>50000</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="17">
         <f>D17/12</f>
         <v>4166.666666666667</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="17">
         <v>1000</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="17">
         <v>50000</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="19" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2506,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2517,7 +2523,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B1" s="1"/>
@@ -2530,7 +2536,7 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B2" t="s">
@@ -2610,77 +2616,100 @@
       <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.09</v>
-      </c>
-      <c r="E4" s="2">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="G4" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="H4" s="7">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I4" s="2">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="J4" s="7">
-        <v>0.06</v>
-      </c>
-      <c r="K4" s="2">
-        <v>5.5E-2</v>
-      </c>
-      <c r="L4" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="M4" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="N4" s="2">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="O4" s="2">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="P4" s="7">
-        <v>0.09</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="R4" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="S4" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="T4" s="7">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="U4" s="2">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="V4" s="7">
-        <v>0.06</v>
-      </c>
-      <c r="W4" s="2">
-        <v>5.5E-2</v>
-      </c>
-      <c r="X4" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="Y4" s="7">
-        <v>0.05</v>
+      <c r="B4" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="C4" s="6">
+        <f>B4*(1+$B$35)</f>
+        <v>0.23749999999999999</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" ref="D4:Y4" si="0">C4*(1+$B$35)</f>
+        <v>0.22562499999999999</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.21434374999999997</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.20362656249999997</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.19344523437499997</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.18377297265624995</v>
+      </c>
+      <c r="I4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.17458432402343743</v>
+      </c>
+      <c r="J4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.16585510782226556</v>
+      </c>
+      <c r="K4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.15756235243115227</v>
+      </c>
+      <c r="L4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.14968423480959464</v>
+      </c>
+      <c r="M4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.14220002306911489</v>
+      </c>
+      <c r="N4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.13509002191565914</v>
+      </c>
+      <c r="O4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.12833552081987618</v>
+      </c>
+      <c r="P4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.12191874477888236</v>
+      </c>
+      <c r="Q4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.11582280753993823</v>
+      </c>
+      <c r="R4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.11003166716294131</v>
+      </c>
+      <c r="S4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.10453008380479424</v>
+      </c>
+      <c r="T4" s="6">
+        <f t="shared" si="0"/>
+        <v>9.9303579614554521E-2</v>
+      </c>
+      <c r="U4" s="6">
+        <f t="shared" si="0"/>
+        <v>9.4338400633826786E-2</v>
+      </c>
+      <c r="V4" s="6">
+        <f t="shared" si="0"/>
+        <v>8.9621480602135442E-2</v>
+      </c>
+      <c r="W4" s="6">
+        <f t="shared" si="0"/>
+        <v>8.5140406572028662E-2</v>
+      </c>
+      <c r="X4" s="6">
+        <f t="shared" si="0"/>
+        <v>8.0883386243427224E-2</v>
+      </c>
+      <c r="Y4" s="6">
+        <f t="shared" si="0"/>
+        <v>7.6839216931255866E-2</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
@@ -2689,206 +2718,206 @@
       </c>
       <c r="B5">
         <f>1/B4</f>
-        <v>10</v>
-      </c>
-      <c r="C5" s="5">
-        <f t="shared" ref="C5:D5" si="0">1/C4</f>
-        <v>10.526315789473685</v>
-      </c>
-      <c r="D5" s="5">
-        <f t="shared" si="0"/>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="E5" s="5">
-        <f t="shared" ref="E5" si="1">1/E4</f>
-        <v>11.76470588235294</v>
-      </c>
-      <c r="F5" s="5">
-        <f t="shared" ref="F5" si="2">1/F4</f>
-        <v>12.5</v>
-      </c>
-      <c r="G5" s="5">
-        <f t="shared" ref="G5" si="3">1/G4</f>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="H5" s="5">
-        <f t="shared" ref="H5" si="4">1/H4</f>
-        <v>14.285714285714285</v>
-      </c>
-      <c r="I5" s="5">
-        <f t="shared" ref="I5" si="5">1/I4</f>
-        <v>15.384615384615383</v>
-      </c>
-      <c r="J5" s="5">
-        <f t="shared" ref="J5" si="6">1/J4</f>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="K5" s="5">
-        <f t="shared" ref="K5" si="7">1/K4</f>
-        <v>18.181818181818183</v>
-      </c>
-      <c r="L5" s="5">
-        <f t="shared" ref="L5" si="8">1/L4</f>
-        <v>20</v>
-      </c>
-      <c r="M5" s="5">
-        <f t="shared" ref="M5" si="9">1/M4</f>
-        <v>20</v>
-      </c>
-      <c r="N5" s="5">
-        <f t="shared" ref="N5:O5" si="10">1/N4</f>
-        <v>10.526315789473685</v>
-      </c>
-      <c r="O5" s="5">
-        <f t="shared" si="10"/>
-        <v>10.526315789473685</v>
-      </c>
-      <c r="P5" s="5">
-        <f t="shared" ref="P5" si="11">1/P4</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="Q5" s="5">
-        <f t="shared" ref="Q5" si="12">1/Q4</f>
-        <v>11.76470588235294</v>
-      </c>
-      <c r="R5" s="5">
-        <f t="shared" ref="R5" si="13">1/R4</f>
-        <v>12.5</v>
-      </c>
-      <c r="S5" s="5">
-        <f t="shared" ref="S5" si="14">1/S4</f>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="T5" s="5">
-        <f t="shared" ref="T5" si="15">1/T4</f>
-        <v>14.285714285714285</v>
-      </c>
-      <c r="U5" s="5">
-        <f t="shared" ref="U5" si="16">1/U4</f>
-        <v>15.384615384615383</v>
-      </c>
-      <c r="V5" s="5">
-        <f t="shared" ref="V5" si="17">1/V4</f>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="W5" s="5">
-        <f t="shared" ref="W5" si="18">1/W4</f>
-        <v>18.181818181818183</v>
-      </c>
-      <c r="X5" s="5">
-        <f t="shared" ref="X5" si="19">1/X4</f>
-        <v>20</v>
-      </c>
-      <c r="Y5" s="5">
-        <f t="shared" ref="Y5" si="20">1/Y4</f>
-        <v>20</v>
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" ref="C5:D5" si="1">1/C4</f>
+        <v>4.2105263157894735</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="1"/>
+        <v>4.43213296398892</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" ref="E5" si="2">1/E4</f>
+        <v>4.665403119988337</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" ref="F5" si="3">1/F4</f>
+        <v>4.9109506526193023</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" ref="G5" si="4">1/G4</f>
+        <v>5.1694217395992652</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" ref="H5" si="5">1/H4</f>
+        <v>5.441496567999228</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" ref="I5" si="6">1/I4</f>
+        <v>5.7278911242097141</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" ref="J5" si="7">1/J4</f>
+        <v>6.0293590781154887</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" ref="K5" si="8">1/K4</f>
+        <v>6.3466937664373564</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" ref="L5" si="9">1/L4</f>
+        <v>6.6807302804603763</v>
+      </c>
+      <c r="M5" s="4">
+        <f t="shared" ref="M5" si="10">1/M4</f>
+        <v>7.0323476636425024</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" ref="N5:O5" si="11">1/N4</f>
+        <v>7.4024712248868445</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="11"/>
+        <v>7.7920749735651</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" ref="P5" si="12">1/P4</f>
+        <v>8.2021841827001065</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" ref="Q5" si="13">1/Q4</f>
+        <v>8.633878087052743</v>
+      </c>
+      <c r="R5" s="4">
+        <f t="shared" ref="R5" si="14">1/R4</f>
+        <v>9.0882927232134154</v>
+      </c>
+      <c r="S5" s="4">
+        <f t="shared" ref="S5" si="15">1/S4</f>
+        <v>9.5666239191720166</v>
+      </c>
+      <c r="T5" s="4">
+        <f t="shared" ref="T5" si="16">1/T4</f>
+        <v>10.070130441233703</v>
+      </c>
+      <c r="U5" s="4">
+        <f t="shared" ref="U5" si="17">1/U4</f>
+        <v>10.600137306561793</v>
+      </c>
+      <c r="V5" s="4">
+        <f t="shared" ref="V5" si="18">1/V4</f>
+        <v>11.158039270065046</v>
+      </c>
+      <c r="W5" s="4">
+        <f t="shared" ref="W5" si="19">1/W4</f>
+        <v>11.745304494805312</v>
+      </c>
+      <c r="X5" s="4">
+        <f t="shared" ref="X5" si="20">1/X4</f>
+        <v>12.36347841558454</v>
+      </c>
+      <c r="Y5" s="4">
+        <f t="shared" ref="Y5" si="21">1/Y4</f>
+        <v>13.014187805878462</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>0</v>
       </c>
-      <c r="C7" s="5">
-        <f t="shared" ref="C7:H7" si="21">B10</f>
+      <c r="C7" s="4">
+        <f t="shared" ref="C7:H7" si="22">B10</f>
         <v>140</v>
       </c>
-      <c r="D7" s="5">
-        <f t="shared" si="21"/>
-        <v>277.90000000000003</v>
-      </c>
-      <c r="E7" s="5">
-        <f t="shared" si="21"/>
-        <v>416.18500000000006</v>
-      </c>
-      <c r="F7" s="5">
-        <f t="shared" si="21"/>
-        <v>557.1689550000001</v>
-      </c>
-      <c r="G7" s="5">
-        <f t="shared" si="21"/>
-        <v>703.06389300000012</v>
-      </c>
-      <c r="H7" s="5">
-        <f t="shared" si="21"/>
-        <v>856.04003177700019</v>
-      </c>
-      <c r="I7" s="5">
-        <f t="shared" ref="I7:M7" si="22">H10</f>
-        <v>1018.2796347647702</v>
-      </c>
-      <c r="J7" s="5">
+      <c r="D7" s="4">
         <f t="shared" si="22"/>
-        <v>1192.0268561341929</v>
-      </c>
-      <c r="K7" s="5">
+        <v>257.95000000000005</v>
+      </c>
+      <c r="E7" s="4">
         <f t="shared" si="22"/>
-        <v>1379.6354742056051</v>
-      </c>
-      <c r="L7" s="5">
+        <v>363.04603125000006</v>
+      </c>
+      <c r="F7" s="4">
         <f t="shared" si="22"/>
-        <v>1583.6161709189175</v>
-      </c>
-      <c r="M7" s="5">
+        <v>461.58906348925791</v>
+      </c>
+      <c r="G7" s="4">
         <f t="shared" si="22"/>
-        <v>1806.6848619911621</v>
-      </c>
-      <c r="N7" s="5">
-        <f t="shared" ref="N7:T7" si="23">M10</f>
-        <v>2042.7800784792496</v>
-      </c>
-      <c r="O7" s="5">
+        <v>558.0657236033461</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="22"/>
+        <v>655.81649965624297</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" ref="I7:M7" si="23">H10</f>
+        <v>757.45755720955867</v>
+      </c>
+      <c r="J7" s="4">
         <f t="shared" si="23"/>
-        <v>2201.259787378378</v>
-      </c>
-      <c r="P7" s="5">
+        <v>865.15273923681661</v>
+      </c>
+      <c r="K7" s="4">
         <f t="shared" si="23"/>
-        <v>2372.8874292404616</v>
-      </c>
-      <c r="Q7" s="5">
+        <v>980.79296782742949</v>
+      </c>
+      <c r="L7" s="4">
         <f t="shared" si="23"/>
-        <v>2570.5346680048924</v>
-      </c>
-      <c r="R7" s="5">
+        <v>1106.1175683632289</v>
+      </c>
+      <c r="M7" s="4">
         <f t="shared" si="23"/>
-        <v>2796.1428972122344</v>
-      </c>
-      <c r="S7" s="5">
-        <f t="shared" si="23"/>
-        <v>3052.0834355020343</v>
-      </c>
-      <c r="T7" s="5">
-        <f t="shared" si="23"/>
-        <v>3341.179705511503</v>
-      </c>
-      <c r="U7" s="5">
-        <f t="shared" ref="U7:Y7" si="24">T10</f>
-        <v>3666.7398560115889</v>
-      </c>
-      <c r="V7" s="5">
+        <v>1242.7987061515198</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" ref="N7:T7" si="24">M10</f>
+        <v>1392.5021610541532</v>
+      </c>
+      <c r="O7" s="4">
         <f t="shared" si="24"/>
-        <v>4032.5999136475975</v>
-      </c>
-      <c r="W7" s="5">
+        <v>1556.9328299544022</v>
+      </c>
+      <c r="P7" s="4">
         <f t="shared" si="24"/>
-        <v>4443.1779189676445</v>
-      </c>
-      <c r="X7" s="5">
+        <v>1737.8703660036701</v>
+      </c>
+      <c r="Q7" s="4">
         <f t="shared" si="24"/>
-        <v>4903.5398535744398</v>
-      </c>
-      <c r="Y7" s="5">
+        <v>1937.198499788158</v>
+      </c>
+      <c r="R7" s="4">
         <f t="shared" si="24"/>
-        <v>5419.4785186577346</v>
+        <v>2156.9304067682951</v>
+      </c>
+      <c r="S7" s="4">
+        <f t="shared" si="24"/>
+        <v>2399.2317282239173</v>
+      </c>
+      <c r="T7" s="4">
+        <f t="shared" si="24"/>
+        <v>2666.4423622776712</v>
+      </c>
+      <c r="U7" s="4">
+        <f t="shared" ref="U7:Y7" si="25">T10</f>
+        <v>2961.0978207534999</v>
+      </c>
+      <c r="V7" s="4">
+        <f t="shared" si="25"/>
+        <v>3285.9507365000668</v>
+      </c>
+      <c r="W7" s="4">
+        <f t="shared" si="25"/>
+        <v>3643.9929664481565</v>
+      </c>
+      <c r="X7" s="4">
+        <f t="shared" si="25"/>
+        <v>4038.4786438891633</v>
+      </c>
+      <c r="Y7" s="4">
+        <f t="shared" si="25"/>
+        <v>4472.9484736616605</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
@@ -2898,97 +2927,97 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" s="5">
-        <f t="shared" ref="C8:H8" si="25">-B10*C4</f>
-        <v>-13.3</v>
-      </c>
-      <c r="D8" s="5">
-        <f t="shared" si="25"/>
-        <v>-25.011000000000003</v>
-      </c>
-      <c r="E8" s="5">
-        <f t="shared" si="25"/>
-        <v>-35.37572500000001</v>
-      </c>
-      <c r="F8" s="5">
-        <f t="shared" si="25"/>
-        <v>-44.57351640000001</v>
-      </c>
-      <c r="G8" s="5">
-        <f t="shared" si="25"/>
-        <v>-52.729791975000005</v>
-      </c>
-      <c r="H8" s="5">
-        <f t="shared" si="25"/>
-        <v>-59.922802224390018</v>
-      </c>
-      <c r="I8" s="5">
-        <f t="shared" ref="I8:M8" si="26">-H10*I4</f>
-        <v>-66.188176259710062</v>
-      </c>
-      <c r="J8" s="5">
+      <c r="C8" s="4">
+        <f t="shared" ref="C8:H8" si="26">-B10*C4</f>
+        <v>-33.25</v>
+      </c>
+      <c r="D8" s="4">
         <f t="shared" si="26"/>
-        <v>-71.52161136805158</v>
-      </c>
-      <c r="K8" s="5">
+        <v>-58.199968750000011</v>
+      </c>
+      <c r="E8" s="4">
         <f t="shared" si="26"/>
-        <v>-75.879951081308278</v>
-      </c>
-      <c r="L8" s="5">
+        <v>-77.816647760742185</v>
+      </c>
+      <c r="F8" s="4">
         <f t="shared" si="26"/>
-        <v>-79.180808545945879</v>
-      </c>
-      <c r="M8" s="5">
+        <v>-93.991794285911823</v>
+      </c>
+      <c r="G8" s="4">
         <f t="shared" si="26"/>
-        <v>-90.334243099558108</v>
-      </c>
-      <c r="N8" s="5">
-        <f t="shared" ref="N8:T8" si="27">-M10*N4</f>
-        <v>-194.06410745552873</v>
-      </c>
-      <c r="O8" s="5">
+        <v>-107.95515469910323</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="26"/>
+        <v>-120.52134765884429</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" ref="I8:M8" si="27">-H10*I4</f>
+        <v>-132.24021560187498</v>
+      </c>
+      <c r="J8" s="4">
         <f t="shared" si="27"/>
-        <v>-209.1196798009459</v>
-      </c>
-      <c r="P8" s="5">
+        <v>-143.49000084885063</v>
+      </c>
+      <c r="K8" s="4">
         <f t="shared" si="27"/>
-        <v>-213.55986863164154</v>
-      </c>
-      <c r="Q8" s="5">
+        <v>-154.53604725882124</v>
+      </c>
+      <c r="L8" s="4">
         <f t="shared" si="27"/>
-        <v>-218.49544678041588</v>
-      </c>
-      <c r="R8" s="5">
+        <v>-165.5683618298994</v>
+      </c>
+      <c r="M8" s="4">
         <f t="shared" si="27"/>
-        <v>-223.69143177697876</v>
-      </c>
-      <c r="S8" s="5">
-        <f t="shared" si="27"/>
-        <v>-228.90625766265256</v>
-      </c>
-      <c r="T8" s="5">
-        <f t="shared" si="27"/>
-        <v>-233.88257938580523</v>
-      </c>
-      <c r="U8" s="5">
-        <f t="shared" ref="U8:Y8" si="28">-T10*U4</f>
-        <v>-238.33809064075328</v>
-      </c>
-      <c r="V8" s="5">
+        <v>-176.72600468501224</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" ref="N8:T8" si="28">-M10*N4</f>
+        <v>-188.11314745440828</v>
+      </c>
+      <c r="O8" s="4">
         <f t="shared" si="28"/>
-        <v>-241.95599481885586</v>
-      </c>
-      <c r="W8" s="5">
+        <v>-199.80978561376193</v>
+      </c>
+      <c r="P8" s="4">
         <f t="shared" si="28"/>
-        <v>-244.37478554322044</v>
-      </c>
-      <c r="X8" s="5">
+        <v>-211.87897361158434</v>
+      </c>
+      <c r="Q8" s="4">
         <f t="shared" si="28"/>
-        <v>-245.176992678722</v>
-      </c>
-      <c r="Y8" s="5">
+        <v>-224.37176900762088</v>
+      </c>
+      <c r="R8" s="4">
         <f t="shared" si="28"/>
-        <v>-270.97392593288674</v>
+        <v>-237.33064861115668</v>
+      </c>
+      <c r="S8" s="4">
+        <f t="shared" si="28"/>
+        <v>-250.7918936183674</v>
+      </c>
+      <c r="T8" s="4">
+        <f t="shared" si="28"/>
+        <v>-264.78727141006158</v>
+      </c>
+      <c r="U8" s="4">
+        <f t="shared" ref="U8:Y8" si="29">-T10*U4</f>
+        <v>-279.34523253019512</v>
+      </c>
+      <c r="V8" s="4">
+        <f t="shared" si="29"/>
+        <v>-294.49177019081338</v>
+      </c>
+      <c r="W8" s="4">
+        <f t="shared" si="29"/>
+        <v>-310.25104270900886</v>
+      </c>
+      <c r="X8" s="4">
+        <f t="shared" si="29"/>
+        <v>-326.64582798951938</v>
+      </c>
+      <c r="Y8" s="4">
+        <f t="shared" si="29"/>
+        <v>-343.69785809001814</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
@@ -2998,96 +3027,96 @@
       <c r="B9">
         <v>140</v>
       </c>
-      <c r="C9" s="5">
-        <f t="shared" ref="C9:H9" si="29">B9*(1+$B$30)</f>
+      <c r="C9" s="4">
+        <f t="shared" ref="C9:H9" si="30">B9*(1+$B$30)</f>
         <v>151.20000000000002</v>
       </c>
-      <c r="D9" s="5">
-        <f t="shared" si="29"/>
+      <c r="D9" s="4">
+        <f t="shared" si="30"/>
         <v>163.29600000000002</v>
       </c>
-      <c r="E9" s="5">
-        <f t="shared" si="29"/>
+      <c r="E9" s="4">
+        <f t="shared" si="30"/>
         <v>176.35968000000003</v>
       </c>
-      <c r="F9" s="5">
-        <f t="shared" si="29"/>
+      <c r="F9" s="4">
+        <f t="shared" si="30"/>
         <v>190.46845440000004</v>
       </c>
-      <c r="G9" s="5">
-        <f t="shared" si="29"/>
+      <c r="G9" s="4">
+        <f t="shared" si="30"/>
         <v>205.70593075200006</v>
       </c>
-      <c r="H9" s="5">
-        <f t="shared" si="29"/>
+      <c r="H9" s="4">
+        <f t="shared" si="30"/>
         <v>222.16240521216008</v>
       </c>
-      <c r="I9" s="5">
-        <f t="shared" ref="I9:M9" si="30">H9*(1+$B$30)</f>
+      <c r="I9" s="4">
+        <f t="shared" ref="I9:M9" si="31">H9*(1+$B$30)</f>
         <v>239.93539762913289</v>
       </c>
-      <c r="J9" s="5">
-        <f t="shared" si="30"/>
+      <c r="J9" s="4">
+        <f t="shared" si="31"/>
         <v>259.13022943946356</v>
       </c>
-      <c r="K9" s="5">
-        <f t="shared" si="30"/>
+      <c r="K9" s="4">
+        <f t="shared" si="31"/>
         <v>279.86064779462066</v>
       </c>
-      <c r="L9" s="5">
-        <f t="shared" si="30"/>
+      <c r="L9" s="4">
+        <f t="shared" si="31"/>
         <v>302.24949961819033</v>
       </c>
-      <c r="M9" s="5">
-        <f t="shared" si="30"/>
+      <c r="M9" s="4">
+        <f t="shared" si="31"/>
         <v>326.42945958764557</v>
       </c>
-      <c r="N9" s="5">
-        <f t="shared" ref="N9:T9" si="31">M9*(1+$B$30)</f>
+      <c r="N9" s="4">
+        <f t="shared" ref="N9:T9" si="32">M9*(1+$B$30)</f>
         <v>352.54381635465722</v>
       </c>
-      <c r="O9" s="5">
-        <f t="shared" si="31"/>
+      <c r="O9" s="4">
+        <f t="shared" si="32"/>
         <v>380.74732166302982</v>
       </c>
-      <c r="P9" s="5">
-        <f t="shared" si="31"/>
+      <c r="P9" s="4">
+        <f t="shared" si="32"/>
         <v>411.20710739607222</v>
       </c>
-      <c r="Q9" s="5">
-        <f t="shared" si="31"/>
+      <c r="Q9" s="4">
+        <f t="shared" si="32"/>
         <v>444.10367598775804</v>
       </c>
-      <c r="R9" s="5">
-        <f t="shared" si="31"/>
+      <c r="R9" s="4">
+        <f t="shared" si="32"/>
         <v>479.63197006677871</v>
       </c>
-      <c r="S9" s="5">
-        <f t="shared" si="31"/>
+      <c r="S9" s="4">
+        <f t="shared" si="32"/>
         <v>518.002527672121</v>
       </c>
-      <c r="T9" s="5">
-        <f t="shared" si="31"/>
+      <c r="T9" s="4">
+        <f t="shared" si="32"/>
         <v>559.44272988589069</v>
       </c>
-      <c r="U9" s="5">
-        <f t="shared" ref="U9:Y9" si="32">T9*(1+$B$30)</f>
+      <c r="U9" s="4">
+        <f t="shared" ref="U9:Y9" si="33">T9*(1+$B$30)</f>
         <v>604.19814827676203</v>
       </c>
-      <c r="V9" s="5">
-        <f t="shared" si="32"/>
+      <c r="V9" s="4">
+        <f t="shared" si="33"/>
         <v>652.53400013890302</v>
       </c>
-      <c r="W9" s="5">
-        <f t="shared" si="32"/>
+      <c r="W9" s="4">
+        <f t="shared" si="33"/>
         <v>704.73672015001534</v>
       </c>
-      <c r="X9" s="5">
-        <f t="shared" si="32"/>
+      <c r="X9" s="4">
+        <f t="shared" si="33"/>
         <v>761.11565776201667</v>
       </c>
-      <c r="Y9" s="5">
-        <f t="shared" si="32"/>
+      <c r="Y9" s="4">
+        <f t="shared" si="33"/>
         <v>822.0049103829781</v>
       </c>
     </row>
@@ -3095,302 +3124,302 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="5">
-        <f t="shared" ref="B10:H10" si="33">SUM(B7:B9)</f>
+      <c r="B10" s="4">
+        <f t="shared" ref="B10:H10" si="34">SUM(B7:B9)</f>
         <v>140</v>
       </c>
-      <c r="C10" s="5">
-        <f t="shared" si="33"/>
-        <v>277.90000000000003</v>
-      </c>
-      <c r="D10" s="5">
-        <f t="shared" si="33"/>
-        <v>416.18500000000006</v>
-      </c>
-      <c r="E10" s="5">
-        <f t="shared" si="33"/>
-        <v>557.1689550000001</v>
-      </c>
-      <c r="F10" s="5">
-        <f t="shared" si="33"/>
-        <v>703.06389300000012</v>
-      </c>
-      <c r="G10" s="5">
-        <f t="shared" si="33"/>
-        <v>856.04003177700019</v>
-      </c>
-      <c r="H10" s="5">
-        <f t="shared" si="33"/>
-        <v>1018.2796347647702</v>
-      </c>
-      <c r="I10" s="5">
-        <f t="shared" ref="I10:M10" si="34">SUM(I7:I9)</f>
-        <v>1192.0268561341929</v>
-      </c>
-      <c r="J10" s="5">
+      <c r="C10" s="4">
         <f t="shared" si="34"/>
-        <v>1379.6354742056051</v>
-      </c>
-      <c r="K10" s="5">
+        <v>257.95000000000005</v>
+      </c>
+      <c r="D10" s="4">
         <f t="shared" si="34"/>
-        <v>1583.6161709189175</v>
-      </c>
-      <c r="L10" s="5">
+        <v>363.04603125000006</v>
+      </c>
+      <c r="E10" s="4">
         <f t="shared" si="34"/>
-        <v>1806.6848619911621</v>
-      </c>
-      <c r="M10" s="5">
+        <v>461.58906348925791</v>
+      </c>
+      <c r="F10" s="4">
         <f t="shared" si="34"/>
-        <v>2042.7800784792496</v>
-      </c>
-      <c r="N10" s="5">
-        <f t="shared" ref="N10:T10" si="35">SUM(N7:N9)</f>
-        <v>2201.259787378378</v>
-      </c>
-      <c r="O10" s="5">
+        <v>558.0657236033461</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="34"/>
+        <v>655.81649965624297</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="34"/>
+        <v>757.45755720955867</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" ref="I10:M10" si="35">SUM(I7:I9)</f>
+        <v>865.15273923681661</v>
+      </c>
+      <c r="J10" s="4">
         <f t="shared" si="35"/>
-        <v>2372.8874292404616</v>
-      </c>
-      <c r="P10" s="5">
+        <v>980.79296782742949</v>
+      </c>
+      <c r="K10" s="4">
         <f t="shared" si="35"/>
-        <v>2570.5346680048924</v>
-      </c>
-      <c r="Q10" s="5">
+        <v>1106.1175683632289</v>
+      </c>
+      <c r="L10" s="4">
         <f t="shared" si="35"/>
-        <v>2796.1428972122344</v>
-      </c>
-      <c r="R10" s="5">
+        <v>1242.7987061515198</v>
+      </c>
+      <c r="M10" s="4">
         <f t="shared" si="35"/>
-        <v>3052.0834355020343</v>
-      </c>
-      <c r="S10" s="5">
-        <f t="shared" si="35"/>
-        <v>3341.179705511503</v>
-      </c>
-      <c r="T10" s="5">
-        <f t="shared" si="35"/>
-        <v>3666.7398560115889</v>
-      </c>
-      <c r="U10" s="5">
-        <f t="shared" ref="U10" si="36">SUM(U7:U9)</f>
-        <v>4032.5999136475975</v>
-      </c>
-      <c r="V10" s="5">
-        <f t="shared" ref="V10" si="37">SUM(V7:V9)</f>
-        <v>4443.1779189676445</v>
-      </c>
-      <c r="W10" s="5">
-        <f t="shared" ref="W10" si="38">SUM(W7:W9)</f>
-        <v>4903.5398535744398</v>
-      </c>
-      <c r="X10" s="5">
-        <f t="shared" ref="X10" si="39">SUM(X7:X9)</f>
-        <v>5419.4785186577346</v>
-      </c>
-      <c r="Y10" s="5">
-        <f t="shared" ref="Y10" si="40">SUM(Y7:Y9)</f>
-        <v>5970.5095031078254</v>
+        <v>1392.5021610541532</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" ref="N10:T10" si="36">SUM(N7:N9)</f>
+        <v>1556.9328299544022</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="36"/>
+        <v>1737.8703660036701</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="36"/>
+        <v>1937.198499788158</v>
+      </c>
+      <c r="Q10" s="4">
+        <f t="shared" si="36"/>
+        <v>2156.9304067682951</v>
+      </c>
+      <c r="R10" s="4">
+        <f t="shared" si="36"/>
+        <v>2399.2317282239173</v>
+      </c>
+      <c r="S10" s="4">
+        <f t="shared" si="36"/>
+        <v>2666.4423622776712</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" si="36"/>
+        <v>2961.0978207534999</v>
+      </c>
+      <c r="U10" s="4">
+        <f t="shared" ref="U10" si="37">SUM(U7:U9)</f>
+        <v>3285.9507365000668</v>
+      </c>
+      <c r="V10" s="4">
+        <f t="shared" ref="V10" si="38">SUM(V7:V9)</f>
+        <v>3643.9929664481565</v>
+      </c>
+      <c r="W10" s="4">
+        <f t="shared" ref="W10" si="39">SUM(W7:W9)</f>
+        <v>4038.4786438891633</v>
+      </c>
+      <c r="X10" s="4">
+        <f t="shared" ref="X10" si="40">SUM(X7:X9)</f>
+        <v>4472.9484736616605</v>
+      </c>
+      <c r="Y10" s="4">
+        <f t="shared" ref="Y10" si="41">SUM(Y7:Y9)</f>
+        <v>4951.2555259546198</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <f>B10*$B$31</f>
         <v>4200</v>
       </c>
-      <c r="C12" s="9">
-        <f t="shared" ref="C12:N12" si="41">C10*$B$31</f>
-        <v>8337.0000000000018</v>
-      </c>
-      <c r="D12" s="9">
-        <f t="shared" si="41"/>
-        <v>12485.550000000001</v>
-      </c>
-      <c r="E12" s="9">
-        <f t="shared" si="41"/>
-        <v>16715.068650000001</v>
-      </c>
-      <c r="F12" s="9">
-        <f t="shared" si="41"/>
-        <v>21091.916790000003</v>
-      </c>
-      <c r="G12" s="9">
-        <f t="shared" si="41"/>
-        <v>25681.200953310006</v>
-      </c>
-      <c r="H12" s="9">
-        <f t="shared" si="41"/>
-        <v>30548.389042943105</v>
-      </c>
-      <c r="I12" s="9">
-        <f t="shared" si="41"/>
-        <v>35760.805684025785</v>
-      </c>
-      <c r="J12" s="9">
-        <f t="shared" si="41"/>
-        <v>41389.06422616815</v>
-      </c>
-      <c r="K12" s="9">
-        <f t="shared" si="41"/>
-        <v>47508.485127567525</v>
-      </c>
-      <c r="L12" s="9">
-        <f t="shared" si="41"/>
-        <v>54200.545859734862</v>
-      </c>
-      <c r="M12" s="9">
-        <f t="shared" si="41"/>
-        <v>61283.402354377489</v>
-      </c>
-      <c r="N12" s="9">
-        <f t="shared" si="41"/>
-        <v>66037.793621351331</v>
-      </c>
-      <c r="O12" s="9">
-        <f t="shared" ref="O12:Y12" si="42">O10*$B$31</f>
-        <v>71186.622877213842</v>
-      </c>
-      <c r="P12" s="9">
+      <c r="C12" s="8">
+        <f t="shared" ref="C12:N12" si="42">C10*$B$31</f>
+        <v>7738.5000000000018</v>
+      </c>
+      <c r="D12" s="8">
         <f t="shared" si="42"/>
-        <v>77116.040040146778</v>
-      </c>
-      <c r="Q12" s="9">
+        <v>10891.380937500002</v>
+      </c>
+      <c r="E12" s="8">
         <f t="shared" si="42"/>
-        <v>83884.286916367026</v>
-      </c>
-      <c r="R12" s="9">
+        <v>13847.671904677738</v>
+      </c>
+      <c r="F12" s="8">
         <f t="shared" si="42"/>
-        <v>91562.503065061028</v>
-      </c>
-      <c r="S12" s="9">
+        <v>16741.971708100384</v>
+      </c>
+      <c r="G12" s="8">
         <f t="shared" si="42"/>
-        <v>100235.39116534509</v>
-      </c>
-      <c r="T12" s="9">
+        <v>19674.494989687289</v>
+      </c>
+      <c r="H12" s="8">
         <f t="shared" si="42"/>
-        <v>110002.19568034766</v>
-      </c>
-      <c r="U12" s="9">
+        <v>22723.726716286761</v>
+      </c>
+      <c r="I12" s="8">
         <f t="shared" si="42"/>
-        <v>120977.99740942793</v>
-      </c>
-      <c r="V12" s="9">
+        <v>25954.582177104498</v>
+      </c>
+      <c r="J12" s="8">
         <f t="shared" si="42"/>
-        <v>133295.33756902933</v>
-      </c>
-      <c r="W12" s="9">
+        <v>29423.789034822883</v>
+      </c>
+      <c r="K12" s="8">
         <f t="shared" si="42"/>
-        <v>147106.19560723318</v>
-      </c>
-      <c r="X12" s="9">
+        <v>33183.527050896868</v>
+      </c>
+      <c r="L12" s="8">
         <f t="shared" si="42"/>
-        <v>162584.35555973204</v>
-      </c>
-      <c r="Y12" s="9">
+        <v>37283.961184545595</v>
+      </c>
+      <c r="M12" s="8">
         <f t="shared" si="42"/>
-        <v>179115.28509323476</v>
+        <v>41775.064831624601</v>
+      </c>
+      <c r="N12" s="8">
+        <f t="shared" si="42"/>
+        <v>46707.984898632065</v>
+      </c>
+      <c r="O12" s="8">
+        <f t="shared" ref="O12:Y12" si="43">O10*$B$31</f>
+        <v>52136.110980110105</v>
+      </c>
+      <c r="P12" s="8">
+        <f t="shared" si="43"/>
+        <v>58115.954993644737</v>
+      </c>
+      <c r="Q12" s="8">
+        <f t="shared" si="43"/>
+        <v>64707.912203048851</v>
+      </c>
+      <c r="R12" s="8">
+        <f t="shared" si="43"/>
+        <v>71976.951846717522</v>
+      </c>
+      <c r="S12" s="8">
+        <f t="shared" si="43"/>
+        <v>79993.270868330132</v>
+      </c>
+      <c r="T12" s="8">
+        <f t="shared" si="43"/>
+        <v>88832.934622604997</v>
+      </c>
+      <c r="U12" s="8">
+        <f t="shared" si="43"/>
+        <v>98578.522095002001</v>
+      </c>
+      <c r="V12" s="8">
+        <f t="shared" si="43"/>
+        <v>109319.7889934447</v>
+      </c>
+      <c r="W12" s="8">
+        <f t="shared" si="43"/>
+        <v>121154.35931667491</v>
+      </c>
+      <c r="X12" s="8">
+        <f t="shared" si="43"/>
+        <v>134188.45420984982</v>
+      </c>
+      <c r="Y12" s="8">
+        <f t="shared" si="43"/>
+        <v>148537.66577863859</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <f>$B$32</f>
         <v>4000</v>
       </c>
-      <c r="C14" s="9">
-        <f t="shared" ref="C14:Y14" si="43">$B$32</f>
+      <c r="C14" s="8">
+        <f t="shared" ref="C14:Y14" si="44">$B$32</f>
         <v>4000</v>
       </c>
-      <c r="D14" s="9">
-        <f t="shared" si="43"/>
+      <c r="D14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="E14" s="9">
-        <f t="shared" si="43"/>
+      <c r="E14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="F14" s="9">
-        <f t="shared" si="43"/>
+      <c r="F14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="G14" s="9">
-        <f t="shared" si="43"/>
+      <c r="G14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="H14" s="9">
-        <f t="shared" si="43"/>
+      <c r="H14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="I14" s="9">
-        <f t="shared" si="43"/>
+      <c r="I14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="J14" s="9">
-        <f t="shared" si="43"/>
+      <c r="J14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="K14" s="9">
-        <f t="shared" si="43"/>
+      <c r="K14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="L14" s="9">
-        <f t="shared" si="43"/>
+      <c r="L14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="M14" s="9">
-        <f t="shared" si="43"/>
+      <c r="M14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="N14" s="9">
-        <f t="shared" si="43"/>
+      <c r="N14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="O14" s="9">
-        <f t="shared" si="43"/>
+      <c r="O14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="P14" s="9">
-        <f t="shared" si="43"/>
+      <c r="P14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="Q14" s="9">
-        <f t="shared" si="43"/>
+      <c r="Q14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="R14" s="9">
-        <f t="shared" si="43"/>
+      <c r="R14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="S14" s="9">
-        <f t="shared" si="43"/>
+      <c r="S14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="T14" s="9">
-        <f t="shared" si="43"/>
+      <c r="T14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="U14" s="9">
-        <f t="shared" si="43"/>
+      <c r="U14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="V14" s="9">
-        <f t="shared" si="43"/>
+      <c r="V14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="W14" s="9">
-        <f t="shared" si="43"/>
+      <c r="W14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="X14" s="9">
-        <f t="shared" si="43"/>
+      <c r="X14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
-      <c r="Y14" s="9">
-        <f t="shared" si="43"/>
+      <c r="Y14" s="8">
+        <f t="shared" si="44"/>
         <v>4000</v>
       </c>
     </row>
@@ -3398,100 +3427,100 @@
       <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <f>$B$33</f>
         <v>29000</v>
       </c>
-      <c r="C15" s="9">
-        <f t="shared" ref="C15:Y15" si="44">$B$33</f>
+      <c r="C15" s="8">
+        <f t="shared" ref="C15:Y15" si="45">$B$33</f>
         <v>29000</v>
       </c>
-      <c r="D15" s="9">
-        <f t="shared" si="44"/>
+      <c r="D15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="E15" s="9">
-        <f t="shared" si="44"/>
+      <c r="E15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="F15" s="9">
-        <f t="shared" si="44"/>
+      <c r="F15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="G15" s="9">
-        <f t="shared" si="44"/>
+      <c r="G15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="H15" s="9">
-        <f t="shared" si="44"/>
+      <c r="H15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="I15" s="9">
-        <f t="shared" si="44"/>
+      <c r="I15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="J15" s="9">
-        <f t="shared" si="44"/>
+      <c r="J15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="K15" s="9">
-        <f t="shared" si="44"/>
+      <c r="K15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="L15" s="9">
-        <f t="shared" si="44"/>
+      <c r="L15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="M15" s="9">
-        <f t="shared" si="44"/>
+      <c r="M15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="N15" s="9">
-        <f t="shared" si="44"/>
+      <c r="N15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="O15" s="9">
-        <f t="shared" si="44"/>
+      <c r="O15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="P15" s="9">
-        <f t="shared" si="44"/>
+      <c r="P15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="Q15" s="9">
-        <f t="shared" si="44"/>
+      <c r="Q15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="R15" s="9">
-        <f t="shared" si="44"/>
+      <c r="R15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="S15" s="9">
-        <f t="shared" si="44"/>
+      <c r="S15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="T15" s="9">
-        <f t="shared" si="44"/>
+      <c r="T15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="U15" s="9">
-        <f t="shared" si="44"/>
+      <c r="U15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="V15" s="9">
-        <f t="shared" si="44"/>
+      <c r="V15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="W15" s="9">
-        <f t="shared" si="44"/>
+      <c r="W15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="X15" s="9">
-        <f t="shared" si="44"/>
+      <c r="X15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
-      <c r="Y15" s="9">
-        <f t="shared" si="44"/>
+      <c r="Y15" s="8">
+        <f t="shared" si="45"/>
         <v>29000</v>
       </c>
     </row>
@@ -3499,100 +3528,100 @@
       <c r="A16" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <f>SUM(B14:B15)</f>
         <v>33000</v>
       </c>
-      <c r="C16" s="8">
-        <f t="shared" ref="C16:M16" si="45">SUM(C14:C15)</f>
+      <c r="C16" s="7">
+        <f t="shared" ref="C16:M16" si="46">SUM(C14:C15)</f>
         <v>33000</v>
       </c>
-      <c r="D16" s="8">
-        <f t="shared" si="45"/>
-        <v>33000</v>
-      </c>
-      <c r="E16" s="8">
-        <f t="shared" si="45"/>
-        <v>33000</v>
-      </c>
-      <c r="F16" s="8">
-        <f t="shared" si="45"/>
-        <v>33000</v>
-      </c>
-      <c r="G16" s="8">
-        <f t="shared" si="45"/>
-        <v>33000</v>
-      </c>
-      <c r="H16" s="8">
-        <f t="shared" si="45"/>
-        <v>33000</v>
-      </c>
-      <c r="I16" s="8">
-        <f t="shared" si="45"/>
-        <v>33000</v>
-      </c>
-      <c r="J16" s="8">
-        <f t="shared" si="45"/>
-        <v>33000</v>
-      </c>
-      <c r="K16" s="8">
-        <f t="shared" si="45"/>
-        <v>33000</v>
-      </c>
-      <c r="L16" s="8">
-        <f t="shared" si="45"/>
-        <v>33000</v>
-      </c>
-      <c r="M16" s="8">
-        <f t="shared" si="45"/>
-        <v>33000</v>
-      </c>
-      <c r="N16" s="8">
-        <f t="shared" ref="N16:O16" si="46">SUM(N14:N15)</f>
-        <v>33000</v>
-      </c>
-      <c r="O16" s="8">
+      <c r="D16" s="7">
         <f t="shared" si="46"/>
         <v>33000</v>
       </c>
-      <c r="P16" s="8">
-        <f t="shared" ref="P16" si="47">SUM(P14:P15)</f>
+      <c r="E16" s="7">
+        <f t="shared" si="46"/>
         <v>33000</v>
       </c>
-      <c r="Q16" s="8">
-        <f t="shared" ref="Q16" si="48">SUM(Q14:Q15)</f>
+      <c r="F16" s="7">
+        <f t="shared" si="46"/>
         <v>33000</v>
       </c>
-      <c r="R16" s="8">
-        <f t="shared" ref="R16" si="49">SUM(R14:R15)</f>
+      <c r="G16" s="7">
+        <f t="shared" si="46"/>
         <v>33000</v>
       </c>
-      <c r="S16" s="8">
-        <f t="shared" ref="S16" si="50">SUM(S14:S15)</f>
+      <c r="H16" s="7">
+        <f t="shared" si="46"/>
         <v>33000</v>
       </c>
-      <c r="T16" s="8">
-        <f t="shared" ref="T16" si="51">SUM(T14:T15)</f>
+      <c r="I16" s="7">
+        <f t="shared" si="46"/>
         <v>33000</v>
       </c>
-      <c r="U16" s="8">
-        <f t="shared" ref="U16" si="52">SUM(U14:U15)</f>
+      <c r="J16" s="7">
+        <f t="shared" si="46"/>
         <v>33000</v>
       </c>
-      <c r="V16" s="8">
-        <f t="shared" ref="V16" si="53">SUM(V14:V15)</f>
+      <c r="K16" s="7">
+        <f t="shared" si="46"/>
         <v>33000</v>
       </c>
-      <c r="W16" s="8">
-        <f t="shared" ref="W16" si="54">SUM(W14:W15)</f>
+      <c r="L16" s="7">
+        <f t="shared" si="46"/>
         <v>33000</v>
       </c>
-      <c r="X16" s="8">
-        <f t="shared" ref="X16" si="55">SUM(X14:X15)</f>
+      <c r="M16" s="7">
+        <f t="shared" si="46"/>
         <v>33000</v>
       </c>
-      <c r="Y16" s="8">
-        <f t="shared" ref="Y16" si="56">SUM(Y14:Y15)</f>
+      <c r="N16" s="7">
+        <f t="shared" ref="N16:O16" si="47">SUM(N14:N15)</f>
+        <v>33000</v>
+      </c>
+      <c r="O16" s="7">
+        <f t="shared" si="47"/>
+        <v>33000</v>
+      </c>
+      <c r="P16" s="7">
+        <f t="shared" ref="P16" si="48">SUM(P14:P15)</f>
+        <v>33000</v>
+      </c>
+      <c r="Q16" s="7">
+        <f t="shared" ref="Q16" si="49">SUM(Q14:Q15)</f>
+        <v>33000</v>
+      </c>
+      <c r="R16" s="7">
+        <f t="shared" ref="R16" si="50">SUM(R14:R15)</f>
+        <v>33000</v>
+      </c>
+      <c r="S16" s="7">
+        <f t="shared" ref="S16" si="51">SUM(S14:S15)</f>
+        <v>33000</v>
+      </c>
+      <c r="T16" s="7">
+        <f t="shared" ref="T16" si="52">SUM(T14:T15)</f>
+        <v>33000</v>
+      </c>
+      <c r="U16" s="7">
+        <f t="shared" ref="U16" si="53">SUM(U14:U15)</f>
+        <v>33000</v>
+      </c>
+      <c r="V16" s="7">
+        <f t="shared" ref="V16" si="54">SUM(V14:V15)</f>
+        <v>33000</v>
+      </c>
+      <c r="W16" s="7">
+        <f t="shared" ref="W16" si="55">SUM(W14:W15)</f>
+        <v>33000</v>
+      </c>
+      <c r="X16" s="7">
+        <f t="shared" ref="X16" si="56">SUM(X14:X15)</f>
+        <v>33000</v>
+      </c>
+      <c r="Y16" s="7">
+        <f t="shared" ref="Y16" si="57">SUM(Y14:Y15)</f>
         <v>33000</v>
       </c>
     </row>
@@ -3600,591 +3629,591 @@
       <c r="A18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <f>B12-B16</f>
         <v>-28800</v>
       </c>
-      <c r="C18" s="8">
-        <f t="shared" ref="C18:N18" si="57">C12-C16</f>
-        <v>-24663</v>
-      </c>
-      <c r="D18" s="8">
-        <f t="shared" si="57"/>
-        <v>-20514.449999999997</v>
-      </c>
-      <c r="E18" s="8">
-        <f t="shared" si="57"/>
-        <v>-16284.931349999999</v>
-      </c>
-      <c r="F18" s="8">
-        <f t="shared" si="57"/>
-        <v>-11908.083209999997</v>
-      </c>
-      <c r="G18" s="8">
-        <f t="shared" si="57"/>
-        <v>-7318.7990466899937</v>
-      </c>
-      <c r="H18" s="8">
-        <f t="shared" si="57"/>
-        <v>-2451.6109570568951</v>
-      </c>
-      <c r="I18" s="8">
-        <f t="shared" si="57"/>
-        <v>2760.805684025785</v>
-      </c>
-      <c r="J18" s="8">
-        <f t="shared" si="57"/>
-        <v>8389.0642261681496</v>
-      </c>
-      <c r="K18" s="8">
-        <f t="shared" si="57"/>
-        <v>14508.485127567525</v>
-      </c>
-      <c r="L18" s="8">
-        <f t="shared" si="57"/>
-        <v>21200.545859734862</v>
-      </c>
-      <c r="M18" s="8">
-        <f t="shared" si="57"/>
-        <v>28283.402354377489</v>
-      </c>
-      <c r="N18" s="8">
-        <f t="shared" si="57"/>
-        <v>33037.793621351331</v>
-      </c>
-      <c r="O18" s="8">
-        <f t="shared" ref="O18:Y18" si="58">O12-O16</f>
-        <v>38186.622877213842</v>
-      </c>
-      <c r="P18" s="8">
+      <c r="C18" s="7">
+        <f t="shared" ref="C18:N18" si="58">C12-C16</f>
+        <v>-25261.5</v>
+      </c>
+      <c r="D18" s="7">
         <f t="shared" si="58"/>
-        <v>44116.040040146778</v>
-      </c>
-      <c r="Q18" s="8">
+        <v>-22108.619062499998</v>
+      </c>
+      <c r="E18" s="7">
         <f t="shared" si="58"/>
-        <v>50884.286916367026</v>
-      </c>
-      <c r="R18" s="8">
+        <v>-19152.328095322264</v>
+      </c>
+      <c r="F18" s="7">
         <f t="shared" si="58"/>
-        <v>58562.503065061028</v>
-      </c>
-      <c r="S18" s="8">
+        <v>-16258.028291899616</v>
+      </c>
+      <c r="G18" s="7">
         <f t="shared" si="58"/>
-        <v>67235.391165345092</v>
-      </c>
-      <c r="T18" s="8">
+        <v>-13325.505010312711</v>
+      </c>
+      <c r="H18" s="7">
         <f t="shared" si="58"/>
-        <v>77002.195680347664</v>
-      </c>
-      <c r="U18" s="8">
+        <v>-10276.273283713239</v>
+      </c>
+      <c r="I18" s="7">
         <f t="shared" si="58"/>
-        <v>87977.997409427931</v>
-      </c>
-      <c r="V18" s="8">
+        <v>-7045.4178228955025</v>
+      </c>
+      <c r="J18" s="7">
         <f t="shared" si="58"/>
-        <v>100295.33756902933</v>
-      </c>
-      <c r="W18" s="8">
+        <v>-3576.210965177117</v>
+      </c>
+      <c r="K18" s="7">
         <f t="shared" si="58"/>
-        <v>114106.19560723318</v>
-      </c>
-      <c r="X18" s="8">
+        <v>183.52705089686788</v>
+      </c>
+      <c r="L18" s="7">
         <f t="shared" si="58"/>
-        <v>129584.35555973204</v>
-      </c>
-      <c r="Y18" s="8">
+        <v>4283.9611845455947</v>
+      </c>
+      <c r="M18" s="7">
         <f t="shared" si="58"/>
-        <v>146115.28509323476</v>
+        <v>8775.0648316246006</v>
+      </c>
+      <c r="N18" s="7">
+        <f t="shared" si="58"/>
+        <v>13707.984898632065</v>
+      </c>
+      <c r="O18" s="7">
+        <f t="shared" ref="O18:Y18" si="59">O12-O16</f>
+        <v>19136.110980110105</v>
+      </c>
+      <c r="P18" s="7">
+        <f t="shared" si="59"/>
+        <v>25115.954993644737</v>
+      </c>
+      <c r="Q18" s="7">
+        <f t="shared" si="59"/>
+        <v>31707.912203048851</v>
+      </c>
+      <c r="R18" s="7">
+        <f t="shared" si="59"/>
+        <v>38976.951846717522</v>
+      </c>
+      <c r="S18" s="7">
+        <f t="shared" si="59"/>
+        <v>46993.270868330132</v>
+      </c>
+      <c r="T18" s="7">
+        <f t="shared" si="59"/>
+        <v>55832.934622604997</v>
+      </c>
+      <c r="U18" s="7">
+        <f t="shared" si="59"/>
+        <v>65578.522095002001</v>
+      </c>
+      <c r="V18" s="7">
+        <f t="shared" si="59"/>
+        <v>76319.788993444701</v>
+      </c>
+      <c r="W18" s="7">
+        <f t="shared" si="59"/>
+        <v>88154.359316674905</v>
+      </c>
+      <c r="X18" s="7">
+        <f t="shared" si="59"/>
+        <v>101188.45420984982</v>
+      </c>
+      <c r="Y18" s="7">
+        <f t="shared" si="59"/>
+        <v>115537.66577863859</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <f>$B$34</f>
-        <v>100000</v>
-      </c>
-      <c r="C19" s="6">
+        <v>150000</v>
+      </c>
+      <c r="C19" s="5">
         <f>B19+B18</f>
-        <v>71200</v>
-      </c>
-      <c r="D19" s="6">
-        <f t="shared" ref="D19:M19" si="59">C19+C18</f>
-        <v>46537</v>
-      </c>
-      <c r="E19" s="6">
-        <f t="shared" si="59"/>
-        <v>26022.550000000003</v>
-      </c>
-      <c r="F19" s="6">
-        <f t="shared" si="59"/>
-        <v>9737.618650000004</v>
-      </c>
-      <c r="G19" s="6">
-        <f t="shared" si="59"/>
-        <v>-2170.4645599999931</v>
-      </c>
-      <c r="H19" s="6">
-        <f t="shared" si="59"/>
-        <v>-9489.2636066899868</v>
-      </c>
-      <c r="I19" s="6">
-        <f t="shared" si="59"/>
-        <v>-11940.874563746882</v>
-      </c>
-      <c r="J19" s="6">
-        <f t="shared" si="59"/>
-        <v>-9180.0688797210969</v>
-      </c>
-      <c r="K19" s="6">
-        <f t="shared" si="59"/>
-        <v>-791.00465355294727</v>
-      </c>
-      <c r="L19" s="6">
-        <f t="shared" si="59"/>
-        <v>13717.480474014577</v>
-      </c>
-      <c r="M19" s="6">
-        <f t="shared" si="59"/>
-        <v>34918.02633374944</v>
-      </c>
-      <c r="N19" s="6">
+        <v>121200</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" ref="D19:M19" si="60">C19+C18</f>
+        <v>95938.5</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="60"/>
+        <v>73829.880937499998</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="60"/>
+        <v>54677.552842177734</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="60"/>
+        <v>38419.524550278118</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="60"/>
+        <v>25094.019539965408</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" si="60"/>
+        <v>14817.746256252169</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" si="60"/>
+        <v>7772.3284333566662</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" si="60"/>
+        <v>4196.1174681795492</v>
+      </c>
+      <c r="L19" s="5">
+        <f t="shared" si="60"/>
+        <v>4379.6445190764171</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" si="60"/>
+        <v>8663.6057036220118</v>
+      </c>
+      <c r="N19" s="5">
         <f>M19+M18</f>
-        <v>63201.428688126929</v>
-      </c>
-      <c r="O19" s="6">
+        <v>17438.670535246612</v>
+      </c>
+      <c r="O19" s="5">
         <f>N19+N18</f>
-        <v>96239.222309478268</v>
-      </c>
-      <c r="P19" s="6">
-        <f t="shared" ref="P19:Y19" si="60">O19+O18</f>
-        <v>134425.84518669211</v>
-      </c>
-      <c r="Q19" s="6">
-        <f t="shared" si="60"/>
-        <v>178541.88522683887</v>
-      </c>
-      <c r="R19" s="6">
-        <f t="shared" si="60"/>
-        <v>229426.17214320588</v>
-      </c>
-      <c r="S19" s="6">
-        <f t="shared" si="60"/>
-        <v>287988.67520826694</v>
-      </c>
-      <c r="T19" s="6">
-        <f t="shared" si="60"/>
-        <v>355224.06637361203</v>
-      </c>
-      <c r="U19" s="6">
-        <f t="shared" si="60"/>
-        <v>432226.26205395971</v>
-      </c>
-      <c r="V19" s="6">
-        <f t="shared" si="60"/>
-        <v>520204.25946338766</v>
-      </c>
-      <c r="W19" s="6">
-        <f t="shared" si="60"/>
-        <v>620499.59703241696</v>
-      </c>
-      <c r="X19" s="6">
-        <f t="shared" si="60"/>
-        <v>734605.79263965017</v>
-      </c>
-      <c r="Y19" s="6">
-        <f t="shared" si="60"/>
-        <v>864190.14819938224</v>
+        <v>31146.655433878677</v>
+      </c>
+      <c r="P19" s="5">
+        <f t="shared" ref="P19:Y19" si="61">O19+O18</f>
+        <v>50282.766413988778</v>
+      </c>
+      <c r="Q19" s="5">
+        <f t="shared" si="61"/>
+        <v>75398.721407633508</v>
+      </c>
+      <c r="R19" s="5">
+        <f t="shared" si="61"/>
+        <v>107106.63361068236</v>
+      </c>
+      <c r="S19" s="5">
+        <f t="shared" si="61"/>
+        <v>146083.58545739989</v>
+      </c>
+      <c r="T19" s="5">
+        <f t="shared" si="61"/>
+        <v>193076.85632573004</v>
+      </c>
+      <c r="U19" s="5">
+        <f t="shared" si="61"/>
+        <v>248909.79094833502</v>
+      </c>
+      <c r="V19" s="5">
+        <f t="shared" si="61"/>
+        <v>314488.31304333702</v>
+      </c>
+      <c r="W19" s="5">
+        <f t="shared" si="61"/>
+        <v>390808.10203678173</v>
+      </c>
+      <c r="X19" s="5">
+        <f t="shared" si="61"/>
+        <v>478962.4613534566</v>
+      </c>
+      <c r="Y19" s="5">
+        <f t="shared" si="61"/>
+        <v>580150.91556330642</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <f>B16/B10</f>
         <v>235.71428571428572</v>
       </c>
-      <c r="C21" s="6">
-        <f t="shared" ref="C21:N21" si="61">C16/C10</f>
-        <v>118.74775098956458</v>
-      </c>
-      <c r="D21" s="6">
-        <f t="shared" si="61"/>
-        <v>79.291661160301302</v>
-      </c>
-      <c r="E21" s="6">
-        <f t="shared" si="61"/>
-        <v>59.227994854810234</v>
-      </c>
-      <c r="F21" s="6">
-        <f t="shared" si="61"/>
-        <v>46.937412557467226</v>
-      </c>
-      <c r="G21" s="6">
-        <f t="shared" si="61"/>
-        <v>38.549599054961668</v>
-      </c>
-      <c r="H21" s="6">
-        <f t="shared" si="61"/>
-        <v>32.407600892090151</v>
-      </c>
-      <c r="I21" s="6">
-        <f t="shared" si="61"/>
-        <v>27.683940030529826</v>
-      </c>
-      <c r="J21" s="6">
-        <f t="shared" si="61"/>
-        <v>23.919361756772325</v>
-      </c>
-      <c r="K21" s="6">
-        <f t="shared" si="61"/>
-        <v>20.838382813968895</v>
-      </c>
-      <c r="L21" s="6">
-        <f t="shared" si="61"/>
-        <v>18.26549870110188</v>
-      </c>
-      <c r="M21" s="6">
-        <f t="shared" si="61"/>
-        <v>16.154455561641708</v>
-      </c>
-      <c r="N21" s="6">
-        <f t="shared" si="61"/>
-        <v>14.991415456374563</v>
-      </c>
-      <c r="O21" s="6">
-        <f t="shared" ref="O21:Y21" si="62">O16/O10</f>
-        <v>13.907107262379903</v>
-      </c>
-      <c r="P21" s="6">
+      <c r="C21" s="5">
+        <f t="shared" ref="C21:N21" si="62">C16/C10</f>
+        <v>127.93176972281448</v>
+      </c>
+      <c r="D21" s="5">
         <f t="shared" si="62"/>
-        <v>12.837796124964456</v>
-      </c>
-      <c r="Q21" s="6">
+        <v>90.897564384268406</v>
+      </c>
+      <c r="E21" s="5">
         <f t="shared" si="62"/>
-        <v>11.80197193530457</v>
-      </c>
-      <c r="R21" s="6">
+        <v>71.492161773819788</v>
+      </c>
+      <c r="F21" s="5">
         <f t="shared" si="62"/>
-        <v>10.812286327477763</v>
-      </c>
-      <c r="S21" s="6">
+        <v>59.132820032242769</v>
+      </c>
+      <c r="G21" s="5">
         <f t="shared" si="62"/>
-        <v>9.8767510007211694</v>
-      </c>
-      <c r="T21" s="6">
+        <v>50.318953575119707</v>
+      </c>
+      <c r="H21" s="5">
         <f t="shared" si="62"/>
-        <v>8.999820357011906</v>
-      </c>
-      <c r="U21" s="6">
+        <v>43.566797487070552</v>
+      </c>
+      <c r="I21" s="5">
         <f t="shared" si="62"/>
-        <v>8.1833062308803637</v>
-      </c>
-      <c r="V21" s="6">
+        <v>38.143553737240119</v>
+      </c>
+      <c r="J21" s="5">
         <f t="shared" si="62"/>
-        <v>7.4271164922577366</v>
-      </c>
-      <c r="W21" s="6">
+        <v>33.646244500609377</v>
+      </c>
+      <c r="K21" s="5">
         <f t="shared" si="62"/>
-        <v>6.7298321183103305</v>
-      </c>
-      <c r="X21" s="6">
+        <v>29.83407997834404</v>
+      </c>
+      <c r="L21" s="5">
         <f t="shared" si="62"/>
-        <v>6.0891467484169031</v>
-      </c>
-      <c r="Y21" s="6">
+        <v>26.552972606632807</v>
+      </c>
+      <c r="M21" s="5">
         <f t="shared" si="62"/>
-        <v>5.5271664809883534</v>
+        <v>23.698347423043359</v>
+      </c>
+      <c r="N21" s="5">
+        <f t="shared" si="62"/>
+        <v>21.195519398846812</v>
+      </c>
+      <c r="O21" s="5">
+        <f t="shared" ref="O21:Y21" si="63">O16/O10</f>
+        <v>18.988758106213261</v>
+      </c>
+      <c r="P21" s="5">
+        <f t="shared" si="63"/>
+        <v>17.03490891801161</v>
+      </c>
+      <c r="Q21" s="5">
+        <f t="shared" si="63"/>
+        <v>15.299520047771747</v>
+      </c>
+      <c r="R21" s="5">
+        <f t="shared" si="63"/>
+        <v>13.754402966498345</v>
+      </c>
+      <c r="S21" s="5">
+        <f t="shared" si="63"/>
+        <v>12.376041000118018</v>
+      </c>
+      <c r="T21" s="5">
+        <f t="shared" si="63"/>
+        <v>11.144515310744652</v>
+      </c>
+      <c r="U21" s="5">
+        <f t="shared" si="63"/>
+        <v>10.042755551213459</v>
+      </c>
+      <c r="V21" s="5">
+        <f t="shared" si="63"/>
+        <v>9.055999916532631</v>
+      </c>
+      <c r="W21" s="5">
+        <f t="shared" si="63"/>
+        <v>8.1713939604296417</v>
+      </c>
+      <c r="X21" s="5">
+        <f t="shared" si="63"/>
+        <v>7.3776839134892667</v>
+      </c>
+      <c r="Y21" s="5">
+        <f t="shared" si="63"/>
+        <v>6.6649761514050487</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <f>B14/B9</f>
         <v>28.571428571428573</v>
       </c>
-      <c r="C22" s="6">
-        <f t="shared" ref="C22:Y22" si="63">C14/C9</f>
+      <c r="C22" s="5">
+        <f t="shared" ref="C22:Y22" si="64">C14/C9</f>
         <v>26.455026455026452</v>
       </c>
-      <c r="D22" s="6">
-        <f t="shared" si="63"/>
+      <c r="D22" s="5">
+        <f t="shared" si="64"/>
         <v>24.495394865765235</v>
       </c>
-      <c r="E22" s="6">
-        <f t="shared" si="63"/>
+      <c r="E22" s="5">
+        <f t="shared" si="64"/>
         <v>22.680921172004844</v>
       </c>
-      <c r="F22" s="6">
-        <f t="shared" si="63"/>
+      <c r="F22" s="5">
+        <f t="shared" si="64"/>
         <v>21.000852937041522</v>
       </c>
-      <c r="G22" s="6">
-        <f t="shared" si="63"/>
+      <c r="G22" s="5">
+        <f t="shared" si="64"/>
         <v>19.445234200964371</v>
       </c>
-      <c r="H22" s="6">
-        <f t="shared" si="63"/>
+      <c r="H22" s="5">
+        <f t="shared" si="64"/>
         <v>18.004846482374415</v>
       </c>
-      <c r="I22" s="6">
-        <f t="shared" si="63"/>
+      <c r="I22" s="5">
+        <f t="shared" si="64"/>
         <v>16.67115415034668</v>
       </c>
-      <c r="J22" s="6">
-        <f t="shared" si="63"/>
+      <c r="J22" s="5">
+        <f t="shared" si="64"/>
         <v>15.43625384291359</v>
       </c>
-      <c r="K22" s="6">
-        <f t="shared" si="63"/>
+      <c r="K22" s="5">
+        <f t="shared" si="64"/>
         <v>14.292827632327398</v>
       </c>
-      <c r="L22" s="6">
-        <f t="shared" si="63"/>
+      <c r="L22" s="5">
+        <f t="shared" si="64"/>
         <v>13.234099659562405</v>
       </c>
-      <c r="M22" s="6">
-        <f t="shared" si="63"/>
+      <c r="M22" s="5">
+        <f t="shared" si="64"/>
         <v>12.253795981076301</v>
       </c>
-      <c r="N22" s="6">
-        <f t="shared" si="63"/>
+      <c r="N22" s="5">
+        <f t="shared" si="64"/>
         <v>11.346107389885463</v>
       </c>
-      <c r="O22" s="6">
-        <f t="shared" si="63"/>
+      <c r="O22" s="5">
+        <f t="shared" si="64"/>
         <v>10.505654990634687</v>
       </c>
-      <c r="P22" s="6">
-        <f t="shared" si="63"/>
+      <c r="P22" s="5">
+        <f t="shared" si="64"/>
         <v>9.7274583246617485</v>
       </c>
-      <c r="Q22" s="6">
-        <f t="shared" si="63"/>
+      <c r="Q22" s="5">
+        <f t="shared" si="64"/>
         <v>9.0069058561682844</v>
       </c>
-      <c r="R22" s="6">
-        <f t="shared" si="63"/>
+      <c r="R22" s="5">
+        <f t="shared" si="64"/>
         <v>8.3397276446002628</v>
       </c>
-      <c r="S22" s="6">
-        <f t="shared" si="63"/>
+      <c r="S22" s="5">
+        <f t="shared" si="64"/>
         <v>7.7219700412965393</v>
       </c>
-      <c r="T22" s="6">
-        <f t="shared" si="63"/>
+      <c r="T22" s="5">
+        <f t="shared" si="64"/>
         <v>7.1499722604597586</v>
       </c>
-      <c r="U22" s="6">
-        <f t="shared" si="63"/>
+      <c r="U22" s="5">
+        <f t="shared" si="64"/>
         <v>6.6203446856108865</v>
       </c>
-      <c r="V22" s="6">
-        <f t="shared" si="63"/>
+      <c r="V22" s="5">
+        <f t="shared" si="64"/>
         <v>6.1299487829730426</v>
       </c>
-      <c r="W22" s="6">
-        <f t="shared" si="63"/>
+      <c r="W22" s="5">
+        <f t="shared" si="64"/>
         <v>5.6758785027528171</v>
       </c>
-      <c r="X22" s="6">
-        <f t="shared" si="63"/>
+      <c r="X22" s="5">
+        <f t="shared" si="64"/>
         <v>5.2554430581044596</v>
       </c>
-      <c r="Y22" s="6">
-        <f t="shared" si="63"/>
+      <c r="Y22" s="5">
+        <f t="shared" si="64"/>
         <v>4.8661509797263509</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <f>$B$31*B5</f>
-        <v>300</v>
-      </c>
-      <c r="C23" s="6">
-        <f t="shared" ref="C23:N23" si="64">$B$31*C5</f>
-        <v>315.78947368421052</v>
-      </c>
-      <c r="D23" s="6">
-        <f t="shared" si="64"/>
-        <v>333.33333333333331</v>
-      </c>
-      <c r="E23" s="6">
-        <f t="shared" si="64"/>
-        <v>352.94117647058823</v>
-      </c>
-      <c r="F23" s="6">
-        <f t="shared" si="64"/>
-        <v>375</v>
-      </c>
-      <c r="G23" s="6">
-        <f t="shared" si="64"/>
-        <v>400</v>
-      </c>
-      <c r="H23" s="6">
-        <f t="shared" si="64"/>
-        <v>428.57142857142856</v>
-      </c>
-      <c r="I23" s="6">
-        <f t="shared" si="64"/>
-        <v>461.53846153846149</v>
-      </c>
-      <c r="J23" s="6">
-        <f t="shared" si="64"/>
-        <v>500.00000000000006</v>
-      </c>
-      <c r="K23" s="6">
-        <f t="shared" si="64"/>
-        <v>545.4545454545455</v>
-      </c>
-      <c r="L23" s="6">
-        <f t="shared" si="64"/>
-        <v>600</v>
-      </c>
-      <c r="M23" s="6">
-        <f t="shared" si="64"/>
-        <v>600</v>
-      </c>
-      <c r="N23" s="6">
-        <f t="shared" si="64"/>
-        <v>315.78947368421052</v>
-      </c>
-      <c r="O23" s="6">
-        <f t="shared" ref="O23:Y23" si="65">$B$31*O5</f>
-        <v>315.78947368421052</v>
-      </c>
-      <c r="P23" s="6">
+        <v>120</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" ref="C23:N23" si="65">$B$31*C5</f>
+        <v>126.31578947368421</v>
+      </c>
+      <c r="D23" s="5">
         <f t="shared" si="65"/>
-        <v>333.33333333333331</v>
-      </c>
-      <c r="Q23" s="6">
+        <v>132.9639889196676</v>
+      </c>
+      <c r="E23" s="5">
         <f t="shared" si="65"/>
-        <v>352.94117647058823</v>
-      </c>
-      <c r="R23" s="6">
+        <v>139.9620935996501</v>
+      </c>
+      <c r="F23" s="5">
         <f t="shared" si="65"/>
-        <v>375</v>
-      </c>
-      <c r="S23" s="6">
+        <v>147.32851957857906</v>
+      </c>
+      <c r="G23" s="5">
         <f t="shared" si="65"/>
-        <v>400</v>
-      </c>
-      <c r="T23" s="6">
+        <v>155.08265218797794</v>
+      </c>
+      <c r="H23" s="5">
         <f t="shared" si="65"/>
-        <v>428.57142857142856</v>
-      </c>
-      <c r="U23" s="6">
+        <v>163.24489703997685</v>
+      </c>
+      <c r="I23" s="5">
         <f t="shared" si="65"/>
-        <v>461.53846153846149</v>
-      </c>
-      <c r="V23" s="6">
+        <v>171.83673372629141</v>
+      </c>
+      <c r="J23" s="5">
         <f t="shared" si="65"/>
-        <v>500.00000000000006</v>
-      </c>
-      <c r="W23" s="6">
+        <v>180.88077234346466</v>
+      </c>
+      <c r="K23" s="5">
         <f t="shared" si="65"/>
-        <v>545.4545454545455</v>
-      </c>
-      <c r="X23" s="6">
+        <v>190.4008129931207</v>
+      </c>
+      <c r="L23" s="5">
         <f t="shared" si="65"/>
-        <v>600</v>
-      </c>
-      <c r="Y23" s="6">
+        <v>200.42190841381128</v>
+      </c>
+      <c r="M23" s="5">
         <f t="shared" si="65"/>
-        <v>600</v>
+        <v>210.97042990927508</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" si="65"/>
+        <v>222.07413674660535</v>
+      </c>
+      <c r="O23" s="5">
+        <f t="shared" ref="O23:Y23" si="66">$B$31*O5</f>
+        <v>233.76224920695302</v>
+      </c>
+      <c r="P23" s="5">
+        <f t="shared" si="66"/>
+        <v>246.06552548100319</v>
+      </c>
+      <c r="Q23" s="5">
+        <f t="shared" si="66"/>
+        <v>259.01634261158227</v>
+      </c>
+      <c r="R23" s="5">
+        <f t="shared" si="66"/>
+        <v>272.64878169640247</v>
+      </c>
+      <c r="S23" s="5">
+        <f t="shared" si="66"/>
+        <v>286.99871757516053</v>
+      </c>
+      <c r="T23" s="5">
+        <f t="shared" si="66"/>
+        <v>302.10391323701106</v>
+      </c>
+      <c r="U23" s="5">
+        <f t="shared" si="66"/>
+        <v>318.00411919685376</v>
+      </c>
+      <c r="V23" s="5">
+        <f t="shared" si="66"/>
+        <v>334.74117810195139</v>
+      </c>
+      <c r="W23" s="5">
+        <f t="shared" si="66"/>
+        <v>352.35913484415937</v>
+      </c>
+      <c r="X23" s="5">
+        <f t="shared" si="66"/>
+        <v>370.90435246753617</v>
+      </c>
+      <c r="Y23" s="5">
+        <f t="shared" si="66"/>
+        <v>390.42563417635387</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
     </row>
     <row r="29" spans="1:25" ht="24" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4192,7 +4221,7 @@
       <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <v>0.08</v>
       </c>
     </row>
@@ -4200,7 +4229,7 @@
       <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>30</v>
       </c>
     </row>
@@ -4208,7 +4237,7 @@
       <c r="A32" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>4000</v>
       </c>
     </row>
@@ -4224,12 +4253,20 @@
       <c r="A34" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="6">
-        <v>100000</v>
+      <c r="B34" s="5">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="27">
+        <v>-0.05</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="11" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>